<commit_message>
Test skeleton for record formatter view helper (refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -262,12 +262,6 @@
     <t xml:space="preserve">Test Titel (PPN)</t>
   </si>
   <si>
-    <t xml:space="preserve">Deutsche Bezeichnung des Metadatenfeldes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Englische Bezeichnung des Metadatenfeldes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anzuzeigende Information in Vollanzeige</t>
   </si>
   <si>
@@ -287,12 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">PPN eines Beispieltitels.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hier steht die deutsche Bezeichnung des Metadaten-Feldes in der Vollanzeige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hier steht die englische Bezeichnung des Metadaten-Feldes in der Vollanzeige</t>
   </si>
   <si>
     <t xml:space="preserve">Die erwartete Anzeige zum angegebenen Testdatensatz</t>
@@ -397,12 +385,6 @@
   </si>
   <si>
     <t xml:space="preserve">3x 084 $2 = rvk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sachgebiete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
   </si>
   <si>
     <t xml:space="preserve">79.65 Lebenslanges Lernen</t>
@@ -517,7 +499,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,20 +550,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FFFF"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FF99"/>
-        <bgColor rgb="FF66FF66"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF66FF66"/>
-        <bgColor rgb="FF66FF99"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -666,7 +636,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -759,14 +729,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -815,15 +777,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -857,7 +815,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FF99FFFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFD99694"/>
       <rgbColor rgb="FF0066CC"/>
@@ -879,8 +837,8 @@
       <rgbColor rgb="FFCC66FF"/>
       <rgbColor rgb="FFF6B26B"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF66FF99"/>
       <rgbColor rgb="FF66FF66"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -906,8 +864,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -918,7 +876,8 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.4604651162791"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4325581395349"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.246511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1039,8 +998,6 @@
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
@@ -1048,8 +1005,6 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
@@ -1061,44 +1016,34 @@
       <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="15"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1110,47 +1055,37 @@
     <row r="20" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="E20" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="20"/>
+        <v>25</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
@@ -1158,19 +1093,15 @@
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
@@ -1178,8 +1109,6 @@
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1200,8 +1129,8 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1221,70 +1150,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
+        <v>29</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="155.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="B2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
+        <v>31</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+        <v>33</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
@@ -1293,61 +1222,61 @@
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>40</v>
+      <c r="A8" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="33"/>
+      <c r="A9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="31"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="A10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -1357,49 +1286,35 @@
       <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="35" t="n">
+      <c r="A14" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="33" t="n">
         <v>868759473</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39" t="s">
-        <v>49</v>
+      <c r="C14" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test for bibliographic citations (refs #120, refs #150)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Basisklassifikation" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -391,6 +392,34 @@
   </si>
   <si>
     <t xml:space="preserve">/vufind/Search/Results?lookfor=“Lebenslanges+Lernen“&amp;type=bklname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliographische Zitate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige des Felds Bibliografische Zitate (PICA-Feld 2277).
+Dient der Identifikation und dem Nachweis von alten Drucken und wird auch für die Suche verwendet.
+Anzeige des Felds:
+Bibliografische Zitate: 510a
+Bibliographic citations: 510a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliographic (Name of source)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">510 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliographisches Zitat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBN On-line IT\ICCU\MODE\018621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VD17 3:009152Z</t>
   </si>
 </sst>
 </file>
@@ -400,7 +429,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -472,13 +501,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -689,10 +711,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,7 +723,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,7 +759,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,7 +779,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,11 +795,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -864,20 +886,20 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.4604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4325581395349"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.5627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1016,7 +1038,7 @@
       <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1024,22 +1046,22 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
@@ -1053,62 +1075,62 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1135,14 +1157,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1581395348837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.4604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,24 +1174,24 @@
       <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" customFormat="false" ht="155.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1178,20 +1200,20 @@
       <c r="B3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -1200,43 +1222,43 @@
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="3"/>
@@ -1244,37 +1266,37 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="30"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
@@ -1286,7 +1308,7 @@
       <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -1299,21 +1321,21 @@
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="33" t="n">
+      <c r="B14" s="32" t="n">
         <v>868759473</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="35" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1332,4 +1354,200 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" customFormat="false" ht="128.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="32" t="n">
+        <v>151797196</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="32" t="n">
+        <v>193804867</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="Ticket #150"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test for fingerprints; made testing more precise (refs #120, refs #149, refs #97)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Basisklassifikation" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -388,7 +389,8 @@
     <t xml:space="preserve">3x 084 $2 = rvk</t>
   </si>
   <si>
-    <t xml:space="preserve">79.65 Lebenslanges Lernen</t>
+    <t xml:space="preserve">79.65 Lebenslanges Lernen
+81.92 Berufliche Weiterbildung</t>
   </si>
   <si>
     <t xml:space="preserve">/vufind/Search/Results?lookfor=“Lebenslanges+Lernen“&amp;type=bklname</t>
@@ -420,6 +422,27 @@
   </si>
   <si>
     <t xml:space="preserve">VD17 3:009152Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fingerprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fingerprint bei alten Drucken mit Herkunftsangabe aus Pica-Feld 2275 mit Unterfeld $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fingerprint Identifier (Unparsed fingerprint, Institution to which field applies)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">026 $e $5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.ME u-r- m-r- siRe 3 1700R (UFB Erfurt/Gotha; NLB Hannover; Bibliothek des Herzog Anton Ulrich-Museums Braunschweig; SBB-PK Berlin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t,n, o-s- e-n- Dese C 1539A (SBB; ThULB Jena; Wartburg-Stiftung Eisenach)</t>
   </si>
 </sst>
 </file>
@@ -886,7 +909,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1151,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1363,7 +1386,7 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1550,4 +1573,200 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="32" t="n">
+        <v>151797196</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="32" t="n">
+        <v>770927416</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="Ticket #149"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test for Languages metadata (refs #120, refs #134)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Basisklassifikation" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -443,6 +444,27 @@
   </si>
   <si>
     <t xml:space="preserve">t,n, o-s- e-n- Dese C 1539A (SBB; ThULB Jena; Wartburg-Stiftung Eisenach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprachangaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die einzelnen Sprachen (Marc 041a) werden nacheinander angezeigt und durch ein Komma getrennt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">546 $a-$3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">041 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deutsch, Französisch</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1196,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1769,4 +1791,186 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="32" t="n">
+        <v>786233990</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="Ticket #134"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added testing of metadata titles in different languages (refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -60,13 +60,13 @@
     <t xml:space="preserve">Ungefähre Entsprechung  Marc</t>
   </si>
   <si>
-    <t xml:space="preserve">Testkennung Anzeige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testkennung Indexierung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
+    <t xml:space="preserve">Deutsche Bezeichnung in Vollanzeige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Englische Bezeichnung in Vollanzeige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anforderung in Redmine</t>
   </si>
   <si>
     <t xml:space="preserve">Datenfelder</t>
@@ -265,10 +265,13 @@
     <t xml:space="preserve">Test Titel (PPN)</t>
   </si>
   <si>
-    <t xml:space="preserve">Anzuzeigende Information in Vollanzeige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzuzeigende Information in der Kurzanzeige</t>
+    <t xml:space="preserve">Anzuzeigende Information in Vollanzeige (de)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzuzeigende Information in Vollanzeige (en)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzuzeigende Information in der Kurzanzeige (de)</t>
   </si>
   <si>
     <t xml:space="preserve">enthaltener Link</t>
@@ -286,7 +289,10 @@
     <t xml:space="preserve">PPN eines Beispieltitels.</t>
   </si>
   <si>
-    <t xml:space="preserve">Die erwartete Anzeige zum angegebenen Testdatensatz</t>
+    <t xml:space="preserve">Die erwartete deutsche Anzeige zum angegebenen Testdatensatz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die erwartete englische Anzeige zum angegebenen Testdatensatz (optional)</t>
   </si>
   <si>
     <t xml:space="preserve">Wenn der Eintrag in der Such-Ergebnisliste bei dem einzelnen Eintrag angezeigt werden soll, steht hier die Darstellung für das angegebene Exemplar</t>
@@ -360,7 +366,10 @@
     <t xml:space="preserve">Other Classification Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Anforderung in Redmine</t>
+    <t xml:space="preserve">Sachgebiete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket #97</t>
@@ -385,6 +394,9 @@
   </si>
   <si>
     <t xml:space="preserve">Titel der Klassifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzuzeigende Information in der Kurzanzeige</t>
   </si>
   <si>
     <t xml:space="preserve">3x 084 $2 = rvk</t>
@@ -410,6 +422,12 @@
     <t xml:space="preserve">Bibliographic (Name of source)</t>
   </si>
   <si>
+    <t xml:space="preserve">Bibliografische Zitate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliographic citations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ticket #150</t>
   </si>
   <si>
@@ -455,6 +473,12 @@
     <t xml:space="preserve">Language Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprache(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language(s)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ticket #134</t>
   </si>
   <si>
@@ -465,6 +489,9 @@
   </si>
   <si>
     <t xml:space="preserve">Deutsch, Französisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">German, French</t>
   </si>
 </sst>
 </file>
@@ -474,7 +501,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -504,6 +531,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -566,7 +600,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,7 +652,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FF66"/>
-        <bgColor rgb="FF99CC00"/>
+        <bgColor rgb="FF99FF33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF33"/>
+        <bgColor rgb="FF66FF66"/>
       </patternFill>
     </fill>
     <fill>
@@ -703,7 +743,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -728,6 +768,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -768,7 +812,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,6 +836,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -800,11 +848,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,7 +872,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -840,15 +888,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -905,7 +961,7 @@
       <rgbColor rgb="FFF6B26B"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF66FF66"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF99FF33"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -929,22 +985,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0744186046512"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.5627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.5627906976744"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -956,6 +1012,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -984,9 +1041,10 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
@@ -994,6 +1052,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -1002,115 +1061,129 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="212.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+      <c r="A18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>20</v>
+      <c r="A19" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1118,64 +1191,73 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="19" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>24</v>
       </c>
+      <c r="E20" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1194,22 +1276,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2232558139535"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,179 +1300,214 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" customFormat="false" ht="155.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>8</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="32"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="29" t="s">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="B10" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="32" t="n">
+      <c r="E13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="34" t="n">
         <v>868759473</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
+      <c r="C15" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="Ticket #97"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #97"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1406,22 +1524,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3348837209302"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,163 +1547,194 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" customFormat="false" ht="128.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>50</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>8</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="32" t="n">
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="34" t="n">
         <v>151797196</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="32" t="n">
+      <c r="C13" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="34" t="n">
         <v>193804867</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C14" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="Ticket #150"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #150"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1602,22 +1751,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7116279069767"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,163 +1774,194 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+        <v>59</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>8</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="32" t="n">
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="34" t="n">
         <v>151797196</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-    </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="32" t="n">
+      <c r="C13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="34" t="n">
         <v>770927416</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C14" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="Ticket #149"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #149"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1798,22 +1978,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,149 +2002,180 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+        <v>65</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+        <v>66</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>67</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>8</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="32" t="n">
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="34" t="n">
         <v>786233990</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C13" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="Ticket #134"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #134"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Test and fix for minor undefined index problem for zdb number metadata (refs #120, refs #132)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="82">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -492,6 +493,27 @@
   </si>
   <si>
     <t xml:space="preserve">German, French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZDB-Nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazeige der ZDB-Nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Control Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZDB-Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">035 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1393051-5</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1548,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2185,4 +2207,216 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #132"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test and minor fix for publication information (fixes #119, refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Publikationsangaben" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="92">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -498,7 +499,7 @@
     <t xml:space="preserve">ZDB-Nummer</t>
   </si>
   <si>
-    <t xml:space="preserve">Nazeige der ZDB-Nummer</t>
+    <t xml:space="preserve">Anzeige der ZDB-Nummer</t>
   </si>
   <si>
     <t xml:space="preserve">System Control Number</t>
@@ -514,6 +515,37 @@
   </si>
   <si>
     <t xml:space="preserve">1393051-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publikationsangaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Publikationsangaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production, Publication, Distribution, Manufacture, and Copyright Notice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264 $a, $b und $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darstellung im Format „264a [; 264a[...]] : 264b, 264c“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halle (Saale) : Dt. Akad. der Naturforscher Leopoldina, 2012
+Stuttgart : Wiss. Verl.-Ges., 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York ; Geneva : UNITED Nations, 2015</t>
   </si>
 </sst>
 </file>
@@ -2216,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2419,4 +2451,232 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>728470527</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="34" t="n">
+        <v>855352329</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #119"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed unnecessary parantheses, added test case (fixes #149, refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="93">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -309,9 +309,6 @@
     <t xml:space="preserve">Vergleichswert für den Test.</t>
   </si>
   <si>
-    <t xml:space="preserve">Beginnt der Vergleichswert mit den Zeichen „!=“ gilt der Test als erfüllte wenn sich die generierte Anzeige und der Vergleichswert unterscheiden.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jede Zeile beschreibt einen Testfall. Die Testdaten müssen dabei entweder per PPN-Referenz angegeben werden.</t>
   </si>
   <si>
@@ -464,6 +461,12 @@
   </si>
   <si>
     <t xml:space="preserve">t,n, o-s- e-n- Dese C 1539A (SBB; ThULB Jena; Wartburg-Stiftung Eisenach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">026 $e, ohne $5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMUM s.m, m.it quRe 3 1779R 1,1</t>
   </si>
   <si>
     <t xml:space="preserve">Sprachangaben</t>
@@ -1041,8 +1044,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1280,9 +1283,7 @@
     <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
@@ -1298,7 +1299,7 @@
     <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
@@ -1354,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1368,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -1382,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1396,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -1410,7 +1411,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -1424,7 +1425,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1460,13 +1461,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>39</v>
       </c>
       <c r="D9" s="32"/>
       <c r="F9" s="3"/>
@@ -1475,10 +1476,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>41</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
@@ -1488,10 +1489,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>43</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
@@ -1523,7 +1524,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
@@ -1541,18 +1542,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="34" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="36"/>
       <c r="F15" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1601,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1615,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -1629,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1643,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -1657,7 +1658,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -1671,7 +1672,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1707,10 +1708,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>55</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -1742,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -1760,13 +1761,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -1774,13 +1775,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>193804867</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="36"/>
@@ -1805,10 +1806,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1828,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1842,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -1856,7 +1857,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1870,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -1884,7 +1885,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -1898,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1934,10 +1935,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -1969,7 +1970,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -1987,13 +1988,13 @@
     </row>
     <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2001,17 +2002,31 @@
     </row>
     <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>770927416</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="34" t="n">
+        <v>194273989</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2056,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2070,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2084,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2098,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2112,7 +2127,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2126,7 +2141,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2162,7 +2177,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="32"/>
@@ -2195,7 +2210,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -2213,16 +2228,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="37"/>
@@ -2270,7 +2285,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2284,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2298,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2312,7 +2327,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2326,7 +2341,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2340,7 +2355,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2376,7 +2391,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="32"/>
@@ -2409,7 +2424,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -2427,13 +2442,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2460,7 +2475,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2482,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2496,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2510,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2524,7 +2539,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2538,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2552,7 +2567,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2588,10 +2603,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="40"/>
@@ -2623,7 +2638,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -2641,13 +2656,13 @@
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>728470527</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2655,13 +2670,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>855352329</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="36"/>

</xml_diff>

<commit_message>
Translation fix and unit test for numbering metadata (refs #131, refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Publikationsangaben" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Erscheinungsverlauf" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="102">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -549,6 +550,34 @@
   </si>
   <si>
     <t xml:space="preserve">New York ; Geneva : UNITED Nations, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langewiesen : Linus Wittich, 1994-
+Langewiesen : Inform-Verl, 1994-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erscheinungsverlauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige des Erscheinungsverlaufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dates of Publication and/or Sequential Designation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">262 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angaben zur Zählung von fortlaufenden Ressourcen (PICA 4025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1996/97; 2.1999; 3.2001 - 10.2010[?]; auch mit durchgehender Nr.-Zählung</t>
   </si>
 </sst>
 </file>
@@ -800,7 +829,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -962,6 +991,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1044,8 +1077,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1333,8 +1366,8 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1581,7 +1614,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2050,7 +2083,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2473,10 +2506,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2682,6 +2715,20 @@
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
     </row>
+    <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="41" t="n">
+        <v>537824324</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="Ticket #119"/>
@@ -2694,4 +2741,220 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #131"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Translation fix and unit test for numbering pecularities metadata (refs #133, refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Publikationsangaben" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Erscheinungsverlauf" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -579,13 +580,41 @@
   <si>
     <t xml:space="preserve">1.1996/97; 2.1999; 3.2001 - 10.2010[?]; auch mit durchgehender Nr.-Zählung</t>
   </si>
+  <si>
+    <t xml:space="preserve">Anmerkungen zum Erscheinungsverlauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Anmerkungen zum Erscheinungsverlauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbering Peculiarities Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbering peculiarities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">515 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkungen zur Zählung von fortlaufenden Ressourcen; ist in Pica 4225 nicht wiederholbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008 nicht ersch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersch. unregelmäßig</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -829,7 +858,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,6 +1025,10 @@
     </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2750,6 +2783,222 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #131"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
@@ -2772,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2786,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2800,7 +3049,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2814,7 +3063,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2828,7 +3077,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2842,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2878,10 +3127,10 @@
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="40"/>
@@ -2929,25 +3178,39 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>233814418</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>101</v>
+      <c r="C13" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
       <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="34" t="n">
+        <v>502081112</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #131"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #133"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added test for language notes (refs #139, refs #120)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,10 +13,11 @@
     <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Publikationsangaben" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Erscheinungsverlauf" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Angaben über Sprache und Schrift" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="ZDB-Nummer" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Publikationsangaben" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="120">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -499,6 +500,33 @@
   </si>
   <si>
     <t xml:space="preserve">German, French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angaben über Sprache und Schrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entspricht Pica-Feld  4221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">546 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text teilw. dt., teilw. franz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Fraktur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesangstext deutsch, Vorwort, Einleitung und Kritischer Bericht deutsch</t>
   </si>
   <si>
     <t xml:space="preserve">ZDB-Nummer</t>
@@ -1392,6 +1420,236 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="34" t="n">
+        <v>502081112</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #133"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2327,6 +2585,246 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="34" t="n">
+        <v>786233990</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="34" t="n">
+        <v>569359759</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+    </row>
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="34" t="n">
+        <v>849562740</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #139"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2351,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2365,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2379,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2393,7 +2891,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2407,7 +2905,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2421,7 +2919,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2457,7 +2955,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="32"/>
@@ -2508,13 +3006,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2534,7 +3032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2563,7 +3061,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2577,7 +3075,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2591,7 +3089,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2605,7 +3103,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2619,7 +3117,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2633,7 +3131,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2669,10 +3167,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="40"/>
@@ -2722,13 +3220,13 @@
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>728470527</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2736,13 +3234,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>855352329</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="36"/>
@@ -2750,13 +3248,13 @@
     </row>
     <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B15" s="41" t="n">
         <v>537824324</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="36"/>
@@ -2776,7 +3274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2805,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2819,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2833,7 +3331,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2847,7 +3345,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2861,7 +3359,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2875,7 +3373,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2911,10 +3409,10 @@
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="40"/>
@@ -2964,13 +3462,13 @@
     </row>
     <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="36"/>
@@ -2990,234 +3488,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H65536"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-    </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="34" t="n">
-        <v>233814418</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="34" t="n">
-        <v>502081112</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #133"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Metadata for physical descriptions is now generated with the raw Marc record and not token from the index fields (fixes #128)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="Publikationsangaben" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Umfang" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="143">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -635,6 +636,75 @@
   <si>
     <t xml:space="preserve">Ersch. unregelmäßig</t>
   </si>
+  <si>
+    <t xml:space="preserve">Umfang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Umfangsangaben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a,$b,$c und $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a, $b, $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 S. : Ill., graph. Darst. ; 30 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 2x$a, $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Mikrofiches : 219 Bl. : graph. Darst.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 CD-ROM ; 12 cm, in Behältnis 19 x 14 x 2 cm ; 1 Beih. (44 S.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a, $c, $e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Online-Ressource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a, $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62 Bl ; 19 x 17 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a, $e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 S. ; Chorpartitur, 6 St.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Karte : farbig ; 56 x 58 cm, auf Blatt 60 x 76 cm, gefaltet 23 x 11 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 DVD-Video (7 Min.) : s/w, stumm ; 12 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 $a, $b, $c, $e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 CD : digital ; 22 cm ; 1 Blatt</t>
+  </si>
 </sst>
 </file>
 
@@ -644,7 +714,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -674,13 +744,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -735,12 +798,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -886,7 +943,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -911,10 +968,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -955,7 +1008,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -991,11 +1044,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1015,7 +1068,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,7 +1084,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,23 +1092,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1138,20 +1187,20 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.5627906976744"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="45.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1195,7 +1244,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
@@ -1215,34 +1264,34 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="212.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1250,8 +1299,8 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1259,8 +1308,8 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1268,8 +1317,8 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1277,63 +1326,63 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3"/>
@@ -1345,73 +1394,73 @@
       <c r="H19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1427,21 +1476,21 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,12 +1500,12 @@
       <c r="B1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -1465,12 +1514,12 @@
       <c r="B2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1479,12 +1528,12 @@
       <c r="B3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1493,12 +1542,12 @@
       <c r="B4" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1507,12 +1556,12 @@
       <c r="B5" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -1521,118 +1570,118 @@
       <c r="B6" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <v>502081112</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1642,7 +1691,349 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>509133061</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="33" t="n">
+        <v>585243190</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="33" t="n">
+        <v>839312644</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="33" t="n">
+        <v>349876193</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="33" t="n">
+        <v>129495476</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="33" t="n">
+        <v>336079826</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="33" t="n">
+        <v>787199796</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="36"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="33" t="n">
+        <v>872316203</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="33" t="n">
+        <v>683536028</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="33" t="n">
+        <v>826257127</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #128"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1657,21 +2048,21 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,26 +2072,26 @@
       <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1709,12 +2100,12 @@
       <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1723,12 +2114,12 @@
       <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1737,12 +2128,12 @@
       <c r="B5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -1751,132 +2142,132 @@
       <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="31"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="34" t="n">
+      <c r="B15" s="33" t="n">
         <v>868759473</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1890,7 +2281,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1905,20 +2296,20 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,12 +2319,12 @@
       <c r="B1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -1942,12 +2333,12 @@
       <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1956,12 +2347,12 @@
       <c r="B3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1970,12 +2361,12 @@
       <c r="B4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1984,12 +2375,12 @@
       <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -1998,118 +2389,118 @@
       <c r="B6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>151797196</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <v>193804867</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2117,7 +2508,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2132,20 +2523,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7116279069767"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,12 +2546,12 @@
       <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -2169,12 +2560,12 @@
       <c r="B2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -2183,12 +2574,12 @@
       <c r="B3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2197,12 +2588,12 @@
       <c r="B4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2211,12 +2602,12 @@
       <c r="B5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -2225,132 +2616,132 @@
       <c r="B6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>151797196</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <v>770927416</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="34" t="n">
+      <c r="B15" s="33" t="n">
         <v>194273989</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2358,7 +2749,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2373,21 +2764,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,12 +2788,12 @@
       <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -2411,12 +2802,12 @@
       <c r="B2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -2425,12 +2816,12 @@
       <c r="B3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2439,12 +2830,12 @@
       <c r="B4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2453,12 +2844,12 @@
       <c r="B5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -2467,104 +2858,104 @@
       <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2572,7 +2963,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2587,21 +2978,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,12 +3002,12 @@
       <c r="B1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -2625,12 +3016,12 @@
       <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -2639,12 +3030,12 @@
       <c r="B3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2653,12 +3044,12 @@
       <c r="B4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2667,12 +3058,12 @@
       <c r="B5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -2681,130 +3072,130 @@
       <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <v>569359759</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="34" t="n">
+      <c r="B15" s="33" t="n">
         <v>849562740</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2812,7 +3203,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2827,21 +3218,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,12 +3242,12 @@
       <c r="B1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -2865,12 +3256,12 @@
       <c r="B2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -2879,12 +3270,12 @@
       <c r="B3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2893,12 +3284,12 @@
       <c r="B4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2907,12 +3298,12 @@
       <c r="B5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -2921,102 +3312,102 @@
       <c r="B6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3024,7 +3415,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3039,21 +3430,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3063,12 +3454,12 @@
       <c r="B1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -3077,12 +3468,12 @@
       <c r="B2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -3091,12 +3482,12 @@
       <c r="B3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -3105,12 +3496,12 @@
       <c r="B4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -3119,12 +3510,12 @@
       <c r="B5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -3133,132 +3524,132 @@
       <c r="B6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>728470527</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <v>855352329</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="41" t="n">
+      <c r="B15" s="33" t="n">
         <v>537824324</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3266,7 +3657,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3281,21 +3672,21 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8511627906977"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.0976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.6093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="16.7348837209302"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,12 +3696,12 @@
       <c r="B1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -3319,12 +3710,12 @@
       <c r="B2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -3333,12 +3724,12 @@
       <c r="B3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -3347,12 +3738,12 @@
       <c r="B4" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -3361,12 +3752,12 @@
       <c r="B5" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -3375,104 +3766,104 @@
       <c r="B6" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3482,7 +3873,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added cartographic information in the metadata of the full record view (fixes #146)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,9 @@
     <sheet name="Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Umfang" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Maßstab bei Karten" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Projektion bei Karten" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Koordinaten bei Karten" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="165">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -705,6 +708,72 @@
   <si>
     <t xml:space="preserve">1 CD : digital ; 22 cm ; 1 Blatt</t>
   </si>
+  <si>
+    <t xml:space="preserve">Maßstab bei Karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige des Karten-Maßstabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement of scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maßstab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:25.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektion bei Karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Karten-Projektion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement of projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255 $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTM-Abb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koordinaten bei Karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Karten-Koordinaten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement of coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koordinaten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(E 010 30--E 010 40/N 051 12--N 051 06).</t>
+  </si>
 </sst>
 </file>
 
@@ -714,7 +783,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -798,6 +867,12 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -943,7 +1018,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1108,6 +1183,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1187,20 +1266,20 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="45.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.7953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1460,7 +1539,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1476,21 +1555,21 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,7 +1770,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1706,21 +1785,21 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,7 +2112,643 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>470336242</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #146"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>470336242</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #146"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>470336242</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #146"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2048,21 +2763,21 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2996,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2296,20 +3011,20 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +3223,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2523,20 +3238,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,7 +3464,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2764,21 +3479,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,7 +3678,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2978,21 +3693,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,7 +3918,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3218,21 +3933,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3415,7 +4130,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3430,21 +4145,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3657,7 +4372,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3672,21 +4387,21 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="16.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3873,7 +4588,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added custom linking mechanism for related items in metadata including page size (refs #117, refs #163)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <sheet name="Maßstab bei Karten" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Projektion bei Karten" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Koordinaten bei Karten" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Ähnliche Datensätze" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -57,8 +58,33 @@
 </comments>
 </file>
 
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="172">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -774,6 +800,27 @@
   <si>
     <t xml:space="preserve">(E 010 30--E 010 40/N 051 12--N 051 06).</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ähnliche Datensätze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige von Zählung-, Band- und Seitenangaben bei unselbständigen Ressourcen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host Item Entry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">773 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In: Hermes (1991), p. 173-213</t>
+  </si>
 </sst>
 </file>
 
@@ -783,7 +830,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -867,12 +914,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1183,8 +1224,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1259,27 +1300,77 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3885840</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9781560" cy="9524520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.7953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.0232558139535"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1354,7 +1445,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="212.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="212.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1472,7 +1563,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17"/>
       <c r="B20" s="18" t="s">
         <v>22</v>
@@ -1502,7 +1593,7 @@
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -1518,7 +1609,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="17"/>
       <c r="B24" s="18" t="s">
         <v>29</v>
@@ -1539,12 +1630,13 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1553,26 +1645,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1586,7 +1678,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1600,7 +1692,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1614,7 +1706,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1628,7 +1720,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +1734,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1656,7 +1748,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -1666,7 +1758,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1773,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>116</v>
       </c>
@@ -1694,7 +1786,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1704,7 +1796,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1724,7 +1816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1734,7 +1826,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>116</v>
       </c>
@@ -1748,7 +1840,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>116</v>
       </c>
@@ -1762,8 +1854,6 @@
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="Ticket #133"/>
@@ -1783,26 +1873,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1906,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1830,7 +1920,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1844,7 +1934,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1948,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1962,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1886,7 +1976,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -1896,7 +1986,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -1911,7 +2001,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>124</v>
       </c>
@@ -1924,7 +2014,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1934,7 +2024,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1954,7 +2044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1964,7 +2054,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>125</v>
       </c>
@@ -1978,7 +2068,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>127</v>
       </c>
@@ -1992,7 +2082,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
         <v>129</v>
       </c>
@@ -2006,7 +2096,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="36"/>
     </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -2020,7 +2110,7 @@
       <c r="E16" s="35"/>
       <c r="F16" s="36"/>
     </row>
-    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="32" t="s">
         <v>133</v>
       </c>
@@ -2034,7 +2124,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="36"/>
     </row>
-    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="32" t="s">
         <v>135</v>
       </c>
@@ -2048,7 +2138,7 @@
       <c r="E18" s="35"/>
       <c r="F18" s="36"/>
     </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
         <v>137</v>
       </c>
@@ -2062,7 +2152,7 @@
       <c r="E19" s="35"/>
       <c r="F19" s="36"/>
     </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="32" t="s">
         <v>125</v>
       </c>
@@ -2076,7 +2166,7 @@
       <c r="E20" s="35"/>
       <c r="F20" s="36"/>
     </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32" t="s">
         <v>125</v>
       </c>
@@ -2090,7 +2180,7 @@
       <c r="E21" s="35"/>
       <c r="F21" s="36"/>
     </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="32" t="s">
         <v>141</v>
       </c>
@@ -2104,8 +2194,6 @@
       <c r="E22" s="35"/>
       <c r="F22" s="36"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="Ticket #128"/>
@@ -2127,24 +2215,24 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2246,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2172,7 +2260,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2186,7 +2274,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2200,7 +2288,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2214,7 +2302,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2228,7 +2316,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2238,7 +2326,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -2253,7 +2341,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>149</v>
       </c>
@@ -2264,7 +2352,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -2274,7 +2362,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2304,8 +2392,8 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>149</v>
       </c>
       <c r="B13" s="33" t="n">
@@ -2343,20 +2431,20 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2370,7 +2458,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2384,7 +2472,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2398,7 +2486,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2412,7 +2500,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2514,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2528,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2450,7 +2538,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -2465,7 +2553,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>156</v>
       </c>
@@ -2476,7 +2564,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -2486,7 +2574,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2506,7 +2594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2516,8 +2604,8 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>156</v>
       </c>
       <c r="B13" s="33" t="n">
@@ -2552,23 +2640,23 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2582,7 +2670,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2684,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2610,7 +2698,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2624,7 +2712,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2726,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2740,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2662,7 +2750,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -2677,7 +2765,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>163</v>
       </c>
@@ -2688,7 +2776,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -2698,7 +2786,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2718,7 +2806,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2728,8 +2816,8 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B13" s="33" t="n">
@@ -2756,31 +2844,201 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.22790697674419"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="41"/>
+    </row>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>605825009</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2794,7 +3052,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="156.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2808,7 +3066,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2822,7 +3080,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2836,7 +3094,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2850,7 +3108,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2864,7 +3122,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2874,7 +3132,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -2889,7 +3147,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>36</v>
       </c>
@@ -2904,7 +3162,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
         <v>39</v>
       </c>
@@ -2917,7 +3175,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
         <v>41</v>
       </c>
@@ -2930,7 +3188,7 @@
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -2940,7 +3198,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -2960,7 +3218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -2970,7 +3228,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="58.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
         <v>44</v>
       </c>
@@ -2986,7 +3244,6 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C9:C11"/>
@@ -3015,19 +3272,19 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3041,7 +3298,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3055,7 +3312,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3069,7 +3326,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3083,7 +3340,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3097,7 +3354,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3111,7 +3368,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -3121,7 +3378,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -3136,7 +3393,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>53</v>
       </c>
@@ -3149,7 +3406,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3159,7 +3416,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3179,7 +3436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3189,7 +3446,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>53</v>
       </c>
@@ -3203,7 +3460,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>53</v>
       </c>
@@ -3242,19 +3499,19 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3268,7 +3525,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3282,7 +3539,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3296,7 +3553,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3310,7 +3567,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3324,7 +3581,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3338,7 +3595,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -3348,7 +3605,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -3363,7 +3620,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>61</v>
       </c>
@@ -3376,7 +3633,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3386,7 +3643,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3406,7 +3663,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3416,7 +3673,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>61</v>
       </c>
@@ -3430,7 +3687,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>61</v>
       </c>
@@ -3444,7 +3701,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
         <v>64</v>
       </c>
@@ -3480,23 +3737,23 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3510,7 +3767,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3524,7 +3781,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3538,7 +3795,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3552,7 +3809,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3566,7 +3823,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3580,7 +3837,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -3590,7 +3847,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -3605,7 +3862,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>72</v>
       </c>
@@ -3616,7 +3873,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3626,7 +3883,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3646,7 +3903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3656,7 +3913,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>73</v>
       </c>
@@ -3697,20 +3954,20 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3724,7 +3981,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3738,7 +3995,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3752,7 +4009,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3766,7 +4023,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3780,7 +4037,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3794,7 +4051,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -3804,7 +4061,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -3819,7 +4076,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>72</v>
       </c>
@@ -3830,7 +4087,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3840,7 +4097,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3860,7 +4117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3870,7 +4127,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>81</v>
       </c>
@@ -3884,7 +4141,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>81</v>
       </c>
@@ -3898,7 +4155,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
         <v>81</v>
       </c>
@@ -3937,20 +4194,20 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3964,7 +4221,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3978,7 +4235,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -3992,7 +4249,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4006,7 +4263,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4020,7 +4277,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4034,7 +4291,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4044,7 +4301,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -4059,7 +4316,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>90</v>
       </c>
@@ -4070,7 +4327,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4080,7 +4337,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4100,7 +4357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -4110,7 +4367,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>90</v>
       </c>
@@ -4146,23 +4403,23 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4176,7 +4433,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4190,7 +4447,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -4204,7 +4461,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4218,7 +4475,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4232,7 +4489,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4246,7 +4503,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4256,7 +4513,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -4271,7 +4528,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>98</v>
       </c>
@@ -4284,7 +4541,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4294,7 +4551,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4314,7 +4571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -4324,7 +4581,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>98</v>
       </c>
@@ -4338,7 +4595,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
         <v>98</v>
       </c>
@@ -4352,7 +4609,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
         <v>98</v>
       </c>
@@ -4385,26 +4642,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4418,7 +4675,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4432,7 +4689,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -4446,7 +4703,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4460,7 +4717,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4474,7 +4731,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4488,7 +4745,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -4498,7 +4755,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -4513,7 +4770,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
         <v>108</v>
       </c>
@@ -4526,7 +4783,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4536,7 +4793,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4556,7 +4813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
@@ -4566,7 +4823,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>108</v>
       </c>
@@ -4580,8 +4837,6 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="Ticket #131"/>

</xml_diff>

<commit_message>
link to search without redirect to first result item for all but ppn (refs #163)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="173">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -817,6 +817,9 @@
   </si>
   <si>
     <t xml:space="preserve">773 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">773 $g, $i, $t und $w</t>
   </si>
   <si>
     <t xml:space="preserve">In: Hermes (1991), p. 173-213</t>
@@ -1647,7 +1650,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2852,10 +2855,10 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7813953488372"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1162790697674"/>
@@ -2990,13 +2993,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>

</xml_diff>

<commit_message>
Minor fixes and unit test (fixes #137)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,7 @@
     <sheet name="Projektion bei Karten" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Koordinaten bei Karten" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Ähnliche Datensätze" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Teil und Abteilung" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -83,8 +84,33 @@
 </comments>
 </file>
 
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="187">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -428,6 +454,9 @@
     <t xml:space="preserve">Titel der Klassifikation</t>
   </si>
   <si>
+    <t xml:space="preserve">Anzuzeigende Information in der Vollanzeige (de)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anzuzeigende Information in der Kurzanzeige</t>
   </si>
   <si>
@@ -823,6 +852,45 @@
   </si>
   <si>
     <t xml:space="preserve">In: Hermes (1991), p. 173-213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teil und Abteilung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der Bandangabe bzw. um welchen Teil es sich handelt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of part/section of a work; Name of part/section of a work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245 $n $p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Subfelder können mehrfach vorkommen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part 1: Texts, seal impressions, studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19161811X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bd. 1: 1893 bis 1905 ; Halbbd. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serie A: Arbeitshilfen für die Gestaltung der Gottesdienste im Kirchenjahr ; [3]: Perikopenreihe 3 ; Band 2: Sexagesimae bis Jubilate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Teil: 15. und 16. Jahrhundert ; Teilband A</t>
   </si>
 </sst>
 </file>
@@ -833,7 +901,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -917,6 +985,12 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1062,7 +1136,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1231,6 +1305,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1314,9 +1392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3885840</xdr:colOff>
+      <xdr:colOff>3885480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1326,7 +1404,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9781560" cy="9524520"/>
+          <a:ext cx="9943200" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1360,20 +1438,20 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.0232558139535"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.1488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.3767441860465"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1651,20 +1729,20 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -1686,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1700,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1714,7 +1792,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1728,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1742,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1778,10 +1856,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -1799,7 +1877,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1807,13 +1885,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -1831,13 +1909,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -1845,13 +1923,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>502081112</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -1879,20 +1957,20 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -1914,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1928,7 +2006,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1942,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1956,7 +2034,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1970,7 +2048,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2006,10 +2084,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -2027,7 +2105,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2035,13 +2113,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -2059,13 +2137,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>509133061</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2073,13 +2151,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>585243190</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -2087,13 +2165,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>839312644</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -2101,13 +2179,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>349876193</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="35"/>
@@ -2115,13 +2193,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="32" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>129495476</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="35"/>
@@ -2129,13 +2207,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>336079826</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="35"/>
@@ -2143,13 +2221,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>787199796</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
@@ -2157,13 +2235,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>872316203</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="35"/>
@@ -2171,13 +2249,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>683536028</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
@@ -2185,13 +2263,13 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>826257127</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="35"/>
@@ -2219,20 +2297,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2254,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2268,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2282,7 +2360,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2296,7 +2374,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2310,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2346,7 +2424,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2365,7 +2443,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2373,13 +2451,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -2397,13 +2475,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2431,20 +2509,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2466,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2480,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2494,7 +2572,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2508,7 +2586,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2522,7 +2600,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2558,7 +2636,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2577,7 +2655,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2585,13 +2663,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -2609,13 +2687,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2643,20 +2721,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2678,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2692,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2706,7 +2784,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2720,7 +2798,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2734,7 +2812,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2770,7 +2848,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2789,7 +2867,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2797,13 +2875,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -2821,13 +2899,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2854,19 +2932,19 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.47441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2874,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2887,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2895,7 +2973,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,7 +2989,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2924,7 +3002,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2954,12 +3032,12 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
     </row>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2967,13 +3045,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -2993,13 +3071,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3017,6 +3095,223 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.47441860465116"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="41"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>877327637</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="33" t="n">
+        <v>873533267</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="33" t="n">
+        <v>881377961</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #137"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -3024,21 +3319,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,7 +3496,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -3209,13 +3504,13 @@
         <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>18</v>
@@ -3233,18 +3528,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
       <c r="F15" s="36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3272,19 +3567,19 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3292,7 +3587,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -3306,7 +3601,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3320,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -3334,7 +3629,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3348,7 +3643,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -3362,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -3398,10 +3693,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -3419,7 +3714,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3427,13 +3722,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -3451,13 +3746,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -3465,13 +3760,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>193804867</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -3499,19 +3794,19 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -3533,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3547,7 +3842,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -3561,7 +3856,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3575,7 +3870,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -3589,7 +3884,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -3625,10 +3920,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -3646,7 +3941,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3654,13 +3949,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -3678,13 +3973,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -3692,13 +3987,13 @@
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>770927416</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -3706,13 +4001,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>194273989</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -3740,20 +4035,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3761,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -3775,7 +4070,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3789,7 +4084,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -3803,7 +4098,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3817,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -3831,7 +4126,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -3867,7 +4162,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -3886,7 +4181,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3894,13 +4189,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -3918,16 +4213,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
@@ -3954,20 +4249,20 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3975,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -3989,7 +4284,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4003,7 +4298,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4017,7 +4312,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4031,7 +4326,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4045,7 +4340,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4081,7 +4376,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -4100,7 +4395,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4108,13 +4403,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -4132,13 +4427,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -4146,13 +4441,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>569359759</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -4160,13 +4455,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>849562740</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -4194,20 +4489,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4215,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4229,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4243,7 +4538,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4257,7 +4552,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4271,7 +4566,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4285,7 +4580,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4321,7 +4616,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -4340,7 +4635,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4348,13 +4643,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -4372,13 +4667,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -4406,20 +4701,20 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4441,7 +4736,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4455,7 +4750,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4469,7 +4764,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4483,7 +4778,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4497,7 +4792,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4533,10 +4828,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -4554,7 +4849,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4562,13 +4857,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -4586,13 +4881,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>728470527</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -4600,13 +4895,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>855352329</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -4614,13 +4909,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>537824324</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -4648,20 +4943,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4683,7 +4978,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4697,7 +4992,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4711,7 +5006,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4725,7 +5020,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4739,7 +5034,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4775,10 +5070,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -4796,7 +5091,7 @@
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -4804,13 +5099,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>18</v>
@@ -4828,13 +5123,13 @@
     </row>
     <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>

</xml_diff>

<commit_message>
test for online reference/further information metadata (fixes #182)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,6 +24,7 @@
     <sheet name="Koordinaten bei Karten" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Ähnliche Datensätze" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Teil und Abteilung" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Mehr zum Titel" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -109,8 +110,33 @@
 </comments>
 </file>
 
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="195">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -891,6 +917,33 @@
   </si>
   <si>
     <t xml:space="preserve">2. Teil: 15. und 16. Jahrhundert ; Teilband A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehr zum Titel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es werden sämtliche Verknüpfungen aus externen Quellen aus der bibliographischen Ebene (PICA 408X und 4099 in Marc unter 856) dargestellt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Location and Access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket 182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">856 $u $y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inhaltsverzeichnis
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rezension
+Inhaltsverzeichnis
+</t>
   </si>
 </sst>
 </file>
@@ -1392,9 +1445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3885480</xdr:colOff>
+      <xdr:colOff>3885120</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1404,7 +1457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9943200" cy="9524160"/>
+          <a:ext cx="10123920" cy="9523800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1444,14 +1497,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.1488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.3767441860465"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.7348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1734,15 +1787,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,15 +2015,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2302,15 +2355,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,15 +2567,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,15 +2779,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,13 +2991,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3102,19 +3155,19 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3242,7 +3295,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="17" t="s">
         <v>180</v>
       </c>
       <c r="B13" s="33" t="n">
@@ -3256,7 +3309,7 @@
       <c r="F13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="17" t="s">
         <v>180</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -3270,7 +3323,7 @@
       <c r="F14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="17" t="s">
         <v>180</v>
       </c>
       <c r="B15" s="33" t="n">
@@ -3284,7 +3337,7 @@
       <c r="F15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="17" t="s">
         <v>180</v>
       </c>
       <c r="B16" s="33" t="n">
@@ -3300,6 +3353,195 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId2" display="Ticket #137"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="41"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="33" t="n">
+        <v>804999864</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="33" t="n">
+        <v>557127483</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket 182"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3325,15 +3567,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3572,14 +3814,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3799,14 +4041,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,15 +4282,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,15 +4496,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4494,15 +4736,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,15 +4948,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4948,15 +5190,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added dissertation note to the record meta information (fixes #159)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,6 +25,7 @@
     <sheet name="Ähnliche Datensätze" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Teil und Abteilung" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Mehr zum Titel" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Hochschulschriftenvermerk" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -135,8 +136,33 @@
 </comments>
 </file>
 
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="207">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -944,6 +970,42 @@
     <t xml:space="preserve">Rezension
 Inhaltsverzeichnis
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hochschulschriftenvermerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enthält den Hochschulschriftenvermerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dissertation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket 159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502 $a, $b, $c, $d, $g, $o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62295086X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zugl.: Freiburg (Breisgau), Univ., Diss., 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502 $b, $c, $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilitationsschrift, Albert-Ludwigs-Universität Freiburg, 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dissertation, Friedrich-Schiller-Universität Jena, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jena, Univ., Diss., 2015</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1420,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1445,9 +1507,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3885120</xdr:colOff>
+      <xdr:colOff>3884760</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1457,7 +1519,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10123920" cy="9523800"/>
+          <a:ext cx="10304280" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1497,14 +1559,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.7348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1787,15 +1849,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,15 +2077,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,15 +2417,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2567,15 +2629,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,15 +2841,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,13 +3053,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3161,13 +3222,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3372,19 +3432,18 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3510,7 +3569,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B13" s="33" t="n">
@@ -3524,7 +3583,7 @@
       <c r="F13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="17" t="s">
         <v>192</v>
       </c>
       <c r="B14" s="33" t="n">
@@ -3542,6 +3601,222 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId2" display="Ticket 182"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="41"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="33" t="n">
+        <v>617248613</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="33" t="n">
+        <v>881353434</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="33" t="n">
+        <v>839489048</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket 159"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3567,15 +3842,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.6093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,14 +4089,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4041,14 +4316,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,15 +4557,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,15 +4771,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4736,15 +5011,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4948,15 +5223,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,15 +5465,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Show all bibliographic citations in record meta data (fixes #150)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="209">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -556,6 +556,12 @@
     <t xml:space="preserve">VD17 3:009152Z</t>
   </si>
   <si>
+    <t xml:space="preserve">510 $a (wiederholt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IG 1281 ; GW 12189 ; ISTC ih00015000 ; BSB-Ink H-41 ; H 8426</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fingerprint</t>
   </si>
   <si>
@@ -1016,7 +1022,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1100,12 +1106,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1251,7 +1251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1420,10 +1420,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1507,9 +1503,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3884760</xdr:colOff>
+      <xdr:colOff>3884400</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1519,7 +1515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10304280" cy="9523440"/>
+          <a:ext cx="10504080" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1559,14 +1555,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.2093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.6883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.6418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.9953488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1849,15 +1844,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -1879,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1893,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1907,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1921,7 +1915,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1935,7 +1929,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1971,10 +1965,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -2024,13 +2018,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2038,13 +2032,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>502081112</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -2077,15 +2071,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2107,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2121,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2135,7 +2128,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2149,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2163,7 +2156,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2199,10 +2192,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -2252,13 +2245,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>509133061</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2266,13 +2259,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>585243190</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -2280,13 +2273,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>839312644</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -2294,13 +2287,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>349876193</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="35"/>
@@ -2308,13 +2301,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>129495476</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="35"/>
@@ -2322,13 +2315,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>336079826</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="35"/>
@@ -2336,13 +2329,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>787199796</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
@@ -2350,13 +2343,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>872316203</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="35"/>
@@ -2364,13 +2357,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>683536028</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
@@ -2378,13 +2371,13 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="32" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>826257127</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="35"/>
@@ -2417,15 +2410,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2447,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2461,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2475,7 +2467,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2489,7 +2481,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2503,7 +2495,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2539,7 +2531,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2590,13 +2582,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2629,15 +2621,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2659,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2673,7 +2664,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2687,7 +2678,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2701,7 +2692,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2715,7 +2706,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2751,7 +2742,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2802,13 +2793,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2841,15 +2832,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2857,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2871,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2885,7 +2875,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2899,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2913,7 +2903,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2927,7 +2917,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2963,7 +2953,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -3014,13 +3004,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -3053,12 +3043,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3066,7 +3057,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3079,7 +3070,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3087,7 +3078,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,7 +3086,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3103,7 +3094,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3116,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3146,7 +3137,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3185,13 +3176,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3222,12 +3213,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3235,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3248,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3256,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3264,7 +3256,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,7 +3264,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3285,7 +3277,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3315,10 +3307,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C9" s="41"/>
     </row>
@@ -3356,13 +3348,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>877327637</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3370,13 +3362,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3384,13 +3376,13 @@
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -3398,13 +3390,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>881377961</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -3438,12 +3430,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3451,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3464,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3472,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3480,7 +3473,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3501,7 +3494,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3531,7 +3524,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3570,13 +3563,13 @@
     </row>
     <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>804999864</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3584,13 +3577,13 @@
     </row>
     <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>557127483</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3620,18 +3613,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3639,7 +3633,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3652,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3660,7 +3654,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,15 +3662,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>197</v>
+      <c r="B5" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3689,7 +3683,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3719,7 +3713,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3758,13 +3752,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3772,13 +3766,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>617248613</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3786,13 +3780,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>881353434</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -3800,13 +3794,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>839489048</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -3842,15 +3836,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4081,22 +4074,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,6 +4280,20 @@
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
       <c r="F14" s="36"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="33" t="n">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4316,14 +4322,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4331,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4345,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4359,7 +4364,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4373,7 +4378,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4387,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4401,7 +4406,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4437,10 +4442,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -4490,13 +4495,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -4504,13 +4509,13 @@
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>770927416</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -4518,13 +4523,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>194273989</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -4557,15 +4562,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4573,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4587,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4601,7 +4605,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4615,7 +4619,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4629,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4643,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4679,7 +4683,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -4730,16 +4734,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
@@ -4771,15 +4775,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4787,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -4801,7 +4804,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -4815,7 +4818,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -4829,7 +4832,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -4843,7 +4846,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -4857,7 +4860,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4893,7 +4896,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -4944,13 +4947,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -4958,13 +4961,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>569359759</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -4972,13 +4975,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>849562740</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -5011,15 +5014,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5029,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -5041,7 +5043,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -5055,7 +5057,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -5069,7 +5071,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -5083,7 +5085,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -5097,7 +5099,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -5133,7 +5135,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -5184,13 +5186,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -5223,15 +5225,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5239,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -5253,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -5267,7 +5268,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -5281,7 +5282,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -5295,7 +5296,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -5309,7 +5310,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -5345,10 +5346,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -5398,13 +5399,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>728470527</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -5412,13 +5413,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>855352329</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="35"/>
@@ -5426,13 +5427,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>537824324</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="35"/>
@@ -5465,15 +5466,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -5495,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -5509,7 +5509,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -5523,7 +5523,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -5537,7 +5537,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -5551,7 +5551,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -5587,10 +5587,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="38"/>
@@ -5640,13 +5640,13 @@
     </row>
     <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>

</xml_diff>

<commit_message>
Show preceedings and succeding titles in record metadata (fixes #200)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,6 +26,7 @@
     <sheet name="Teil und Abteilung" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Mehr zum Titel" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Hochschulschriftenvermerk" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Vorheriger Späterer Titel" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -161,8 +162,33 @@
 </comments>
 </file>
 
+<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="224">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1013,6 +1039,59 @@
   <si>
     <t xml:space="preserve">Jena, Univ., Diss., 2015</t>
   </si>
+  <si>
+    <t xml:space="preserve">Vorheriger / Späterer Titel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorgänger- und Nachfolger-Verknüpfungen bei fortlaufenden Ressourcen Verknüpfungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preceding Entry, Succeeding Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preceding / Succeeding Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">780 $i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationship information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">780 $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">785 $i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">785 $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">780 $i und $t
+785 $i und $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorg.: Code de procédure civile
+Forts.: Code de procédure civile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">780 $i und $t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorg.: Wirtschaftswoche, der Volkswirt, Aktionär
+Darin aufgeg.: High-Tech &lt;München&gt;
+Darin aufgeg.: Plus
+Darin aufgeg.: Management-Praxis
+Darin aufgeg.: Wirtschaftswoche &lt;Düsseldorf&gt; / Ostausgabe
+1988 Beil. u. 1991 darin aufgeg.: Profitravel
+Darin aufgegangen: Wirtschaftswoche &lt;Düsseldorf&gt; / Green economy. Green economy</t>
+  </si>
 </sst>
 </file>
 
@@ -1022,7 +1101,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1105,6 +1184,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1226,7 +1313,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1250,8 +1337,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1420,14 +1510,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1453,7 +1548,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFD99694"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0563C1"/>
       <rgbColor rgb="FFFFCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1503,9 +1598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3884400</xdr:colOff>
+      <xdr:colOff>3884040</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1515,7 +1610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10504080" cy="9523080"/>
+          <a:ext cx="10694160" cy="9522720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1555,13 +1650,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.6883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.6418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1844,14 +1940,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,14 +2168,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,14 +2508,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,14 +2720,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,14 +2932,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,13 +3144,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3213,13 +3314,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3430,13 +3531,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3619,13 +3720,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3818,6 +3919,237 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.6697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5023255813953"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="33" t="n">
+        <v>130559555</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="33" t="n">
+        <v>129412244</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #200"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -3836,14 +4168,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4076,19 +4409,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,13 +4656,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4562,14 +4897,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4775,14 +5111,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,14 +5351,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5225,14 +5563,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5466,14 +5805,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed title for related items metadata and adjusted relevant marc fields list (fixes #201)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
     <sheet name="Maßstab bei Karten" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Projektion bei Karten" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Koordinaten bei Karten" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Ähnliche Datensätze" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Verwandte Ressourcen" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Teil und Abteilung" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Mehr zum Titel" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Hochschulschriftenvermerk" sheetId="18" state="visible" r:id="rId19"/>
@@ -914,7 +914,7 @@
     <t xml:space="preserve">(E 010 30--E 010 40/N 051 12--N 051 06).</t>
   </si>
   <si>
-    <t xml:space="preserve">Ähnliche Datensätze</t>
+    <t xml:space="preserve">Verwandte Ressourcen</t>
   </si>
   <si>
     <t xml:space="preserve">Anzeige von Zählung-, Band- und Seitenangaben bei unselbständigen Ressourcen</t>
@@ -923,10 +923,10 @@
     <t xml:space="preserve">Host Item Entry </t>
   </si>
   <si>
-    <t xml:space="preserve">Related Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket #117</t>
+    <t xml:space="preserve">Related resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #117, Ticket #201</t>
   </si>
   <si>
     <t xml:space="preserve">773 $g</t>
@@ -1598,9 +1598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3884040</xdr:colOff>
+      <xdr:colOff>3883680</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1610,7 +1610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10694160" cy="9522720"/>
+          <a:ext cx="10893960" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1650,14 +1650,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1940,15 +1940,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,15 +2168,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,15 +2508,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,15 +2720,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,15 +2932,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,19 +3138,19 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3182,7 +3182,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3314,13 +3314,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3531,13 +3531,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3720,13 +3720,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3931,19 +3931,19 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3767441860465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4168,15 +4168,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,14 +4415,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4656,14 +4656,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,15 +4897,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5111,15 +5111,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5351,15 +5351,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5563,15 +5563,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,15 +5805,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Removed failing test due to conversion character conversion
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="222">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -804,12 +804,6 @@
   </si>
   <si>
     <t xml:space="preserve">3 Mikrofiches : 219 Bl. : graph. Darst.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300 $a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 CD-ROM ; 12 cm, in Behältnis 19 x 14 x 2 cm ; 1 Beih. (44 S.)</t>
   </si>
   <si>
     <t xml:space="preserve">300 $a, $c, $e</t>
@@ -1598,9 +1592,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3883680</xdr:colOff>
+      <xdr:colOff>3883320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1610,7 +1604,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10893960" cy="9522360"/>
+          <a:ext cx="11093400" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1650,14 +1644,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="57.9627906976744"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1940,15 +1934,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,23 +2154,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,7 +2368,7 @@
         <v>132</v>
       </c>
       <c r="B15" s="33" t="n">
-        <v>839312644</v>
+        <v>349876193</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>133</v>
@@ -2388,7 +2382,7 @@
         <v>134</v>
       </c>
       <c r="B16" s="33" t="n">
-        <v>349876193</v>
+        <v>129495476</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>135</v>
@@ -2402,7 +2396,7 @@
         <v>136</v>
       </c>
       <c r="B17" s="33" t="n">
-        <v>129495476</v>
+        <v>336079826</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>137</v>
@@ -2416,7 +2410,7 @@
         <v>138</v>
       </c>
       <c r="B18" s="33" t="n">
-        <v>336079826</v>
+        <v>787199796</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>139</v>
@@ -2427,13 +2421,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="33" t="n">
+        <v>872316203</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>140</v>
-      </c>
-      <c r="B19" s="33" t="n">
-        <v>787199796</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>141</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
@@ -2444,10 +2438,10 @@
         <v>128</v>
       </c>
       <c r="B20" s="33" t="n">
-        <v>872316203</v>
+        <v>683536028</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="35"/>
@@ -2455,10 +2449,10 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B21" s="33" t="n">
-        <v>683536028</v>
+        <v>826257127</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>143</v>
@@ -2466,20 +2460,6 @@
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
       <c r="F21" s="36"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22" s="33" t="n">
-        <v>826257127</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2508,15 +2488,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2538,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2552,7 +2532,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2566,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2580,7 +2560,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2594,7 +2574,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2630,7 +2610,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2681,13 +2661,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2720,15 +2700,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2750,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2764,7 +2744,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2778,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2792,7 +2772,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2806,7 +2786,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -2842,7 +2822,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -2893,13 +2873,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -2932,15 +2912,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -2962,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2976,7 +2956,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2990,7 +2970,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3004,7 +2984,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -3018,7 +2998,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -3054,7 +3034,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -3105,13 +3085,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
@@ -3138,19 +3118,19 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3158,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3171,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3179,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3187,7 +3167,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3195,7 +3175,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3208,7 +3188,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3238,7 +3218,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3277,13 +3257,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3314,13 +3294,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3328,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3341,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3349,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,7 +3337,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3345,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3378,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3408,10 +3388,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C9" s="41"/>
     </row>
@@ -3449,13 +3429,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>877327637</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3463,13 +3443,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3477,13 +3457,13 @@
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>873533267</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -3491,13 +3471,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>881377961</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -3531,13 +3511,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3545,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3558,7 +3538,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3566,7 +3546,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3574,7 +3554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3562,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3595,7 +3575,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3625,7 +3605,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3664,13 +3644,13 @@
     </row>
     <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>804999864</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3678,13 +3658,13 @@
     </row>
     <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>557127483</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3720,13 +3700,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3734,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3747,7 +3727,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3755,7 +3735,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3763,7 +3743,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,7 +3751,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3784,7 +3764,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3814,7 +3794,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="41"/>
@@ -3853,13 +3833,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>202</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>204</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3867,13 +3847,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>617248613</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3881,13 +3861,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>881353434</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -3895,13 +3875,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>839489048</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -3937,13 +3917,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3963,7 +3943,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +3951,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,7 +3959,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,7 +3967,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3999,7 +3979,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4024,18 +4004,18 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4044,10 +4024,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4056,7 +4036,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -4114,13 +4094,13 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>130559555</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -4128,13 +4108,13 @@
     </row>
     <row r="18" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -4168,15 +4148,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.0093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,14 +4395,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4656,14 +4636,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,15 +4877,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5111,15 +5091,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5345,21 +5325,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5563,15 +5543,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,15 +5785,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Test for author metadata (refs #243)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Bibliographische Zitate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Fingerprint" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sprachangaben" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Angaben über Sprache und Schrift" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="ZDB-Nummer" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="ZDB-Nummer" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Angaben über Sprache und Schrift" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Publikationsangaben" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Erscheinungsverlauf" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Anmerkungen zum Erscheinungsverlauf" sheetId="10" state="visible" r:id="rId11"/>
@@ -27,6 +27,10 @@
     <sheet name="Mehr zum Titel" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Hochschulschriftenvermerk" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Vorheriger Späterer Titel" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="1. Verfasser" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Körperschaft" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Weitere Verfasser" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Konferenz" sheetId="23" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -187,8 +191,108 @@
 </comments>
 </file>
 
+<file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments22.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments23.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="331">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -645,6 +749,27 @@
     <t xml:space="preserve">German, French</t>
   </si>
   <si>
+    <t xml:space="preserve">ZDB-Nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeige der ZDB-Nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Control Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZDB-Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">035 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1393051-5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Angaben über Sprache und Schrift</t>
   </si>
   <si>
@@ -670,27 +795,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gesangstext deutsch, Vorwort, Einleitung und Kritischer Bericht deutsch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZDB-Nummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzeige der ZDB-Nummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Control Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZDB-Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket #132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">035 $a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1393051-5</t>
   </si>
   <si>
     <t xml:space="preserve">Publikationsangaben</t>
@@ -1085,6 +1189,535 @@
 Darin aufgeg.: Wirtschaftswoche &lt;Düsseldorf&gt; / Ostausgabe
 1988 Beil. u. 1991 darin aufgeg.: Profitravel
 Darin aufgegangen: Wirtschaftswoche &lt;Düsseldorf&gt; / Green economy. Green economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verfasser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darstellung der Verfasserangaben in der Vollanzeige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Entry - Personal Name
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Verfasser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal name
+Person/Familie als 1. geistiger Schöpfer (PICA 3000)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codierte Angaben in $4 werden aufgelöst. 
+Liste englischer Begriffe unter https://www.loc.gov/marc/relators/relacode.html (Marc) und deutscher Begriffe unter https://www.gbv.de/bibliotheken/verbundbibliotheken/02Verbund/01Erschliessung/02Richtlinien/02KatRichtRDA/anhaenge/anhang-beziehungskennzeichen (GBV)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptorzeichen:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1. Verfasser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 100 $a $b ($c, $d) $g [Expansion von $4]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titles and words associated with a name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dates associated with a name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mischellaneus information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relator code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross, Herbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $a, $c und $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">097208612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beerbohm, Max (Sir, 1872-1956)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sherwood, Mary Martha (Mrs, 1775-1851)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $a, $b, $c und $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedikt XVI. (Papst) [InterviewteR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedikt XVI. (Papst) [Interviewee]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 $a und $4
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otte, Volker [ZusammenstellendeR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otte, Volker [Compiler]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Körpereschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darstellung der ersten Körperschaften in der Vollanzeige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heading-Corporate Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Körperschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporate author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporate name or jurisdiction name as entry element</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codierte Angaben in $4 werden aufgelöst. 
+Liste englischer Begriffe unter https://www.loc.gov/marc/relators/relacode.html (Marc) und deutscher Begriffe unter https://www.gbv.de/bibliotheken/verbundbibliotheken/02Verbund/01Erschliessung/02Richtlinien/02KatRichtRDA/anhaenge/anhang-beziehungskennzeichen (GBV)
+710$b ist wiederholbar
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptorzeichen:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1. Verfasser:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 110 $a, $b, $b, ($n, $d, $c) $g [Expansion von $4]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subordinate unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of part/section/meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of meeting or treaty signing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location of meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kognitive Verhaltenstherapie bei medizinisch unerklärten Körperbeschwerden und somatoformen Störungen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $a, $n, $d und $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weimarer Gipstagung, (1, 2011, Weimar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $a, $d und $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">797315829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tagung Umwelt im Wandel - Das Schwarze Dreieck Wird Wieder Bunt, (2014, Görlitz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachtagung "Analysen des FFH-Berichtes 2013 (Art. 17 FFH-RL) und Erörterung der Handlungserfordernisse", (2014, Bonn)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $a, $b, $e und $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen, [VerfasserIn]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen, [Author]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weitere Verfasser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Entry - Personal Name
+Added Entry - Corporate Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other authors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codierte Angaben in $4 werden aufgelöst. 
+Liste englischer Begriffe unter https://www.loc.gov/marc/relators/relacode.html (Marc) und deutscher Begriffe unter https://www.gbv.de/bibliotheken/verbundbibliotheken/02Verbund/01Erschliessung/02Richtlinien/02KatRichtRDA/anhaenge/anhang-beziehungskennzeichen (GBV)
+Wenn mehrere Personen / Körperschaften vorhanden, dann Trennung durch ";"
+710 $b ist wiederholbar
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptorzeichen:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Weitere Verfasser: 700 $a $b ($c, $d) $g [Expansion von $4]; 710 $a, $b, $b, ($n, $d, $c) $g [Expansion von $4] 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $a, $d und $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">521722950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blechinger, Fritz (1954-) [VerfasserIn]; Achtner, Bertram (1960-) [VerfasserIn]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blechinger, Fritz (1954-) [Author]; Achtner, Bertram (1960-) [Author]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $a
+710 $a, $b und $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetLibrary, Inc; University of Virginia, Library, Electronic Text Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $a, $b und $c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">683581341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klemens XI. (Papst)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $a und $4
+710 $a und $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seewald, Peter [InterviewerIn]; Droemer Verlag [Verlag]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seewald, Peter [Interviewer]; Droemer Verlag [Publisher]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 $a
+710 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fischer, Hans-Bertram; F.A. Finger-Institut für Baustoffkunde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 $a und $b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sächsische Landesstiftung Natur und Umwelt, Akademie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konferenzen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angaben zu Kongressen und Konferenzen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Entry-Meeting Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konferenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting name or jurisdiction name as entry element </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">711 ist wiederholbar.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Anzeige:
+Konferenz: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">711 $a ($n, $d, $c)
+                          711 $a ($n, $d, $c)
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">711 $n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711 $d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711 $a, $n, $d und $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wissenschaftliche Tagung der Universitäten Bern und Lausanne (2006.08.29-09.02, Schloss Münchenwiler)
+Colloque organisé par les Universités de Berne et de Lausanne (2006.08.29-09.02, Schloss Münchenwiler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Grenzen der Demokratie (2016.03.09.-11, Aachen)
+The Limits of Democracy (2016.03.09.-11, Aachen)
+Tagung "Die Grenzen der Demokratie" (2016.03.09.-11, Aachen)
+Tagung der DVPW-Themengruppe Politik und Recht (2016.03.09.-11, Aachen)</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1896,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1306,6 +1939,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1335,7 +1975,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1508,6 +2148,30 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1592,9 +2256,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3883320</xdr:colOff>
+      <xdr:colOff>3882960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1604,7 +2268,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11093400" cy="9522000"/>
+          <a:ext cx="11302920" cy="9521640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1644,14 +2308,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.4837209302326"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.2093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1934,15 +2598,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,21 +2820,21 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,15 +3152,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,15 +3364,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,15 +3576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,13 +3788,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3294,13 +3958,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3511,13 +4175,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3700,13 +4364,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3917,13 +4581,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4148,15 +4812,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4382,6 +5046,1251 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="33" t="n">
+        <v>521722950</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B21" s="33" t="n">
+        <v>725223227</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="33" t="n">
+        <v>860726789</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" s="33" t="n">
+        <v>797315829</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C14"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #243"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="F15" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="15"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B26" s="33" t="n">
+        <v>657009032</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" s="33" t="n">
+        <v>875683843</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" s="33" t="n">
+        <v>867529938</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #243"/>
+    <hyperlink ref="F15" r:id="rId3" display="Kognitive Verhaltenstherapie bei medizinisch unerklärten Körperbeschwerden und somatoformen Störungen "/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="45"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="45"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="45"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="45"/>
+      <c r="I14" s="47"/>
+    </row>
+    <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C15" s="45"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" s="45"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="45"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="45"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="45"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" s="45"/>
+    </row>
+    <row r="21" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="B29" s="48" t="n">
+        <v>860726789</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30" s="48" t="n">
+        <v>657009032</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31" s="33" t="n">
+        <v>797315829</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #243"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.4837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.22790697674419"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="94.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="33" t="n">
+        <v>867529938</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" s="33" t="n">
+        <v>881131490</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #244"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -4395,14 +6304,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,14 +6545,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4871,21 +6780,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5048,7 +6957,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
         <v>76</v>
       </c>
@@ -5083,23 +6992,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5135,7 +7044,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -5149,7 +7058,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -5213,7 +7122,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -5267,7 +7176,7 @@
         <v>84</v>
       </c>
       <c r="B13" s="33" t="n">
-        <v>786233990</v>
+        <v>233814418</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>85</v>
@@ -5276,37 +7185,9 @@
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="33" t="n">
-        <v>569359759</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="33" t="n">
-        <v>849562740</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #139"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #132"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5323,23 +7204,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,7 +7228,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -5361,7 +7242,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -5375,7 +7256,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -5403,7 +7284,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -5417,7 +7298,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -5453,7 +7334,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -5504,21 +7385,49 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="33" t="n">
-        <v>233814418</v>
+        <v>786233990</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="35"/>
       <c r="F13" s="36"/>
     </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="33" t="n">
+        <v>569359759</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="33" t="n">
+        <v>849562740</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #132"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #139"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5543,15 +7452,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5785,15 +7694,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixes and unit tests for autho metadata (fixes #243)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1373,7 +1373,7 @@
       </rPr>
       <t xml:space="preserve">Codierte Angaben in $4 werden aufgelöst. 
 Liste englischer Begriffe unter https://www.loc.gov/marc/relators/relacode.html (Marc) und deutscher Begriffe unter https://www.gbv.de/bibliotheken/verbundbibliotheken/02Verbund/01Erschliessung/02Richtlinien/02KatRichtRDA/anhaenge/anhang-beziehungskennzeichen (GBV)
-710$b ist wiederholbar
+110$b ist wiederholbar
 </t>
     </r>
     <r>
@@ -1408,7 +1408,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1. Verfasser:</t>
+      <t xml:space="preserve">Körperschaft:</t>
     </r>
     <r>
       <rPr>
@@ -1418,7 +1418,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> 110 $a, $b, $b, ($n, $d, $c) $g [Expansion von $4]</t>
+      <t xml:space="preserve"> 110 $a, $b, $b, ($c, $d) $g [Expansion von $4]</t>
     </r>
   </si>
   <si>
@@ -1458,7 +1458,7 @@
     <t xml:space="preserve">110 $a, $n, $d und $c</t>
   </si>
   <si>
-    <t xml:space="preserve">Weimarer Gipstagung, (1, 2011, Weimar)</t>
+    <t xml:space="preserve">Weimarer Gipstagung, (Weimar, 2011)</t>
   </si>
   <si>
     <t xml:space="preserve">110 $a, $d und $c</t>
@@ -1467,19 +1467,19 @@
     <t xml:space="preserve">797315829</t>
   </si>
   <si>
-    <t xml:space="preserve">Tagung Umwelt im Wandel - Das Schwarze Dreieck Wird Wieder Bunt, (2014, Görlitz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fachtagung "Analysen des FFH-Berichtes 2013 (Art. 17 FFH-RL) und Erörterung der Handlungserfordernisse", (2014, Bonn)</t>
+    <t xml:space="preserve">Tagung Umwelt im Wandel - Das Schwarze Dreieck Wird Wieder Bunt, (Görlitz, 2014)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachtagung "Analysen  des FFH-Berichtes 2013 (Art. 17 FFH-RL) und Erörterung der Handlungserfordernisse", (Bonn, 2014)</t>
   </si>
   <si>
     <t xml:space="preserve">110 $a, $b, $e und $4</t>
   </si>
   <si>
-    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen, [VerfasserIn]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen, [Author]</t>
+    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen [VerfasserIn]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen [Author]</t>
   </si>
   <si>
     <t xml:space="preserve">Weitere Verfasser</t>
@@ -5053,7 +5053,7 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -5352,8 +5352,8 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5585,7 +5585,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
         <v>272</v>
       </c>
@@ -5599,7 +5599,7 @@
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
         <v>274</v>
       </c>
@@ -5613,7 +5613,7 @@
       <c r="E27" s="21"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
         <v>274</v>
       </c>
@@ -5627,7 +5627,7 @@
       <c r="E28" s="21"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
Show conference information in a records metadata (fixes #244)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="330">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1708,10 +1708,6 @@
   </si>
   <si>
     <t xml:space="preserve">711 $a, $n, $d und $c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wissenschaftliche Tagung der Universitäten Bern und Lausanne (2006.08.29-09.02, Schloss Münchenwiler)
-Colloque organisé par les Universités de Berne et de Lausanne (2006.08.29-09.02, Schloss Münchenwiler)</t>
   </si>
   <si>
     <t xml:space="preserve">Die Grenzen der Demokratie (2016.03.09.-11, Aachen)
@@ -5352,8 +5348,8 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5669,8 +5665,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6049,10 +6045,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6253,7 +6249,7 @@
         <v>328</v>
       </c>
       <c r="B17" s="33" t="n">
-        <v>867529938</v>
+        <v>881131490</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>329</v>
@@ -6262,20 +6258,7 @@
       <c r="E17" s="21"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18" s="33" t="n">
-        <v>881131490</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId2" display="Ticket #244"/>

</xml_diff>

<commit_message>
Fix for special case with with only a and g subfields in Marc fielf 100, 119, 700 or 719 (fixes #243)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="333">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -887,6 +887,15 @@
   </si>
   <si>
     <t xml:space="preserve">Evangelische Kirche in Deutschland, Konferenz für Islamfragen [Author]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 $a, $g und $4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volkshochschule Jena [VerfasserIn]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volkshochschule Jena [Author]</t>
   </si>
   <si>
     <t xml:space="preserve">Weitere Verfasser</t>
@@ -2608,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2621,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2629,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2646,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,7 +2654,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2658,7 +2667,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2688,7 +2697,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -2727,13 +2736,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -2741,13 +2750,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>617248613</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -2755,13 +2764,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>881353434</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
@@ -2769,13 +2778,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>839489048</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
@@ -2827,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -2841,7 +2850,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -2855,7 +2864,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -2869,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -2883,7 +2892,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -2897,7 +2906,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -2933,7 +2942,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -2984,13 +2993,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -3039,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -3053,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3067,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -3081,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3095,7 +3104,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -3109,7 +3118,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -3145,7 +3154,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -3196,13 +3205,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -3251,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -3265,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3279,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -3293,7 +3302,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3307,7 +3316,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -3321,7 +3330,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -3357,7 +3366,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -3408,13 +3417,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>470336242</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -3463,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -3477,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3491,7 +3500,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -3505,7 +3514,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3519,7 +3528,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -3533,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -3569,10 +3578,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
@@ -3622,13 +3631,13 @@
     </row>
     <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -3677,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -3691,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3705,7 +3714,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -3719,7 +3728,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3733,7 +3742,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -3747,7 +3756,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -3783,10 +3792,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
@@ -3836,13 +3845,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -3850,13 +3859,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>502081112</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -3903,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3916,7 +3925,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3924,7 +3933,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,7 +3941,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3940,7 +3949,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -3953,7 +3962,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3983,7 +3992,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -4022,13 +4031,13 @@
     </row>
     <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>804999864</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -4036,13 +4045,13 @@
     </row>
     <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>557127483</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -4092,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4105,7 +4114,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4113,7 +4122,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,7 +4130,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4129,7 +4138,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4142,7 +4151,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4172,7 +4181,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="23"/>
@@ -4211,13 +4220,13 @@
     </row>
     <row r="13" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>605825009</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -4262,7 +4271,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4274,7 +4283,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4291,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4290,7 +4299,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4298,7 +4307,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4310,7 +4319,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4335,18 +4344,18 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4355,10 +4364,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4367,7 +4376,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -4425,13 +4434,13 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>130559555</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -4439,13 +4448,13 @@
     </row>
     <row r="18" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B18" s="24" t="n">
         <v>129412244</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
@@ -4495,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -4509,7 +4518,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -4523,7 +4532,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -4537,7 +4546,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -4551,7 +4560,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -4565,7 +4574,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -4601,10 +4610,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
@@ -4654,13 +4663,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>509133061</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -4668,13 +4677,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>585243190</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -4682,13 +4691,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>349876193</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -4696,13 +4705,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B16" s="24" t="n">
         <v>129495476</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="43"/>
@@ -4710,13 +4719,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>336079826</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="43"/>
@@ -4724,13 +4733,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B18" s="24" t="n">
         <v>787199796</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="43"/>
@@ -4738,13 +4747,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B19" s="24" t="n">
         <v>872316203</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="43"/>
@@ -4752,13 +4761,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B20" s="24" t="n">
         <v>683536028</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="43"/>
@@ -4766,13 +4775,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B21" s="24" t="n">
         <v>826257127</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="43"/>
@@ -5037,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5051,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5065,7 +5074,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5079,7 +5088,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5093,7 +5102,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5107,7 +5116,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5143,10 +5152,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -5196,13 +5205,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -5210,13 +5219,13 @@
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>770927416</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -5224,13 +5233,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>194273989</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -5257,8 +5266,8 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5278,7 +5287,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5292,7 +5301,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5306,7 +5315,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5320,7 +5329,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5334,7 +5343,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5348,7 +5357,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5384,10 +5393,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -5437,13 +5446,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -5451,13 +5460,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>193804867</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -5465,13 +5474,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>409606901</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -5520,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5534,7 +5543,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5548,7 +5557,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5562,7 +5571,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5576,7 +5585,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5590,7 +5599,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5626,7 +5635,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -5677,13 +5686,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -5732,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5746,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5760,7 +5769,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5774,7 +5783,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5788,7 +5797,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5802,7 +5811,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5838,13 +5847,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -5853,10 +5862,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -5866,10 +5875,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -5919,18 +5928,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6254,10 +6263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6546,6 +6555,22 @@
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="24" t="n">
+        <v>848323173</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6591,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6612,7 +6637,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,7 +6645,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6628,7 +6653,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6671,19 +6696,19 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E9" s="28"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>55</v>
@@ -6692,7 +6717,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>57</v>
@@ -6701,7 +6726,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>59</v>
@@ -6710,7 +6735,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>63</v>
@@ -6720,7 +6745,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>61</v>
@@ -6730,7 +6755,7 @@
     </row>
     <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>82</v>
@@ -6739,7 +6764,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>85</v>
@@ -6748,7 +6773,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>87</v>
@@ -6757,7 +6782,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>89</v>
@@ -6766,7 +6791,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>91</v>
@@ -6775,7 +6800,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>61</v>
@@ -6784,7 +6809,7 @@
     </row>
     <row r="21" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>63</v>
@@ -6844,29 +6869,29 @@
     </row>
     <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
@@ -6874,13 +6899,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
@@ -6888,29 +6913,29 @@
     </row>
     <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B29" s="30" t="n">
         <v>860726789</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B30" s="30" t="n">
         <v>657009032</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="21"/>
@@ -6918,13 +6943,13 @@
     </row>
     <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B31" s="24" t="n">
         <v>797315829</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="21"/>
@@ -6972,7 +6997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6985,7 +7010,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6993,7 +7018,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7001,7 +7026,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7009,7 +7034,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -7022,7 +7047,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -7054,20 +7079,20 @@
     </row>
     <row r="9" customFormat="false" ht="94.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>87</v>
@@ -7080,10 +7105,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -7093,7 +7118,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>91</v>
@@ -7154,13 +7179,13 @@
     </row>
     <row r="17" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B17" s="24" t="n">
         <v>881131490</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -7211,7 +7236,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7225,7 +7250,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -7239,7 +7264,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -7253,7 +7278,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7267,7 +7292,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -7281,7 +7306,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -7317,7 +7342,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -7368,16 +7393,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E13" s="43"/>
       <c r="F13" s="44"/>
@@ -7425,7 +7450,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7439,7 +7464,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -7453,7 +7478,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -7467,7 +7492,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7481,7 +7506,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -7495,7 +7520,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -7531,7 +7556,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -7582,13 +7607,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>786233990</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -7596,13 +7621,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>569359759</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -7610,13 +7635,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>849562740</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -7665,7 +7690,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -7679,7 +7704,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -7693,7 +7718,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -7707,7 +7732,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7721,7 +7746,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -7735,7 +7760,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -7771,10 +7796,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
@@ -7824,13 +7849,13 @@
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>728470527</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -7838,13 +7863,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B14" s="24" t="n">
         <v>855352329</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -7852,13 +7877,13 @@
     </row>
     <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>537824324</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>

</xml_diff>

<commit_message>
Replaced bad encodings in unit test fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1038,7 +1038,7 @@
     <t xml:space="preserve">710 $a und $b</t>
   </si>
   <si>
-    <t xml:space="preserve">Sächsische Landesstiftung Natur und Umwelt, Akademie</t>
+    <t xml:space="preserve">Sächsische Landesstiftung Natur und Umwelt, Akademie</t>
   </si>
   <si>
     <t xml:space="preserve">Konferenzen</t>
@@ -6265,8 +6265,8 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6598,8 +6598,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6941,7 +6941,7 @@
       <c r="E30" s="21"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
Replaced another bad encoding in unit test fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -874,7 +874,7 @@
     <t xml:space="preserve">797315829</t>
   </si>
   <si>
-    <t xml:space="preserve">Tagung Umwelt im Wandel - Das Schwarze Dreieck Wird Wieder Bunt, (Görlitz, 2014)</t>
+    <t xml:space="preserve">Tagung Umwelt im Wandel - Das Schwarze Dreieck Wird Wieder Bunt, (Görlitz, 2014)</t>
   </si>
   <si>
     <t xml:space="preserve">Fachtagung "Analysen  des FFH-Berichtes 2013 (Art. 17 FFH-RL) und Erörterung der Handlungserfordernisse", (Bonn, 2014)</t>
@@ -6265,8 +6265,8 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6598,8 +6598,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Changed test cases because of changes in the records
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1399,8 +1399,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Rezension
-Inhaltsverzeichnis
+    <t xml:space="preserve">Inhaltsverzeichnis
+Zentralblatt MATH
 </t>
   </si>
   <si>
@@ -1511,7 +1511,7 @@
     <t xml:space="preserve">300 $a, $c, $e</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Online-Ressource</t>
+    <t xml:space="preserve">Online-Ressource</t>
   </si>
   <si>
     <t xml:space="preserve">300 $c</t>
@@ -2261,9 +2261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3882960</xdr:colOff>
+      <xdr:colOff>3882600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2273,7 +2273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11302920" cy="9521640"/>
+          <a:ext cx="11521440" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2313,14 +2313,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2603,13 +2603,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2820,15 +2820,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,15 +3032,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,15 +3244,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,15 +3456,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,15 +3670,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3892,19 +3892,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4048,7 +4048,7 @@
         <v>242</v>
       </c>
       <c r="B14" s="24" t="n">
-        <v>557127483</v>
+        <v>773516468</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>244</v>
@@ -4087,13 +4087,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4257,13 +4257,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,21 +4482,21 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4814,13 +4814,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5031,14 +5031,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5272,14 +5272,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5513,15 +5513,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5725,15 +5725,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.3627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5972,11 +5972,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6265,17 +6265,17 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6604,11 +6604,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.1023255813954"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6986,10 +6986,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.4837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.47441860465116"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7220,15 +7220,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7434,15 +7434,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7674,15 +7674,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Unit test for item notes (fixes #136)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -26,11 +26,12 @@
     <sheet name="Mehr zum Titel" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Verwandte Ressourcen" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Vorheriger Späterer Titel" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Umfang" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="Fingerprint" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Bibliographische Zitate" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="ZDB-Nummer" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="Basisklassifikation" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Anmerkungen" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Umfang" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Fingerprint" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Bibliographische Zitate" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="ZDB-Nummer" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Basisklassifikation" sheetId="24" state="visible" r:id="rId25"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -142,6 +143,31 @@
 </file>
 
 <file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -292,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="365">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1479,6 +1505,267 @@
 Darin aufgeg.: Wirtschaftswoche &lt;Düsseldorf&gt; / Ostausgabe
 1988 Beil. u. 1991 darin aufgeg.: Profitravel
 Darin aufgegangen: Wirtschaftswoche &lt;Düsseldorf&gt; / Green economy. Green economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkungen und Titelvarianten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varying Form of Title, General notes, With note, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkungen:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note/added entry controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abgebildet werden nur die Einträge, wo der 1. Indikator = 1 ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Allgemeine Anmerkung:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Alle Kategorien sind wiederholbar. Die Darstellung sieht eine Zeile pro Kategorie
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptionszeichen zwischen den Subfeldern:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Subfelder durch : bzw. , getrennt.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Anmerkungen: 264 $i: $a, $f, $g
+                         500 $a
+                         501 $a
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF999999"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptionszeichen zwischen den Subfeldern:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deskriptionszeichen dienen nur der </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verbindung </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">von zwei Subfeldern und werden auch nur dann angezeigt, z.B. $a:_$b -&gt; "Alpha:_Centauri" -&gt; bei $a ohne $b würde </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">kein</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ":_" folgen -&gt; "Alpha", bei $b ohne $a würde auch kein ":_" vorangestellt -&gt; "Centauri"! </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ausnahme: nach $i/$n ohne $a folgt immer ein ":_" (Doppelpunkt Blank) und ersetzt das eigentlich folgende Deskriptionszeichen des nachfolgenden Subfelds</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title proper/short title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $f </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date or sequential designation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">501 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $i, $a
+500 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hauptsacht. Anfangs: Nature and resources
+Zusatz wechselt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $i, $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebent. : Nature, science, progrès 
+Zusatz bis 88.1960: Revue des sciences et de leurs applications  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $i, $a
+500 $a
+501 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zusatz anfangs: a weekly illustrated journal of science
+Zusatz bis 435.2005, Nr. 7039: international weekly journal of science    
+Repr.: New York, NY : Johnson
+Ungezählte Beil.: The genome directory; The yeast genome directory; Suppl.; Produktschau für Deutschland; Science in Spain; Science in Latin America; Nature net guide; Nature jobs; Science &amp; technology networks in Scandinavia; Nature outlook; Nature insight; Nature publishing index  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">246 $a
+500 $a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallelt.:Thuringiæ Tabula
+Titelkartusche mit allegor. Darstell. der Landwirtschaft und der Jagd unten rechts. - Paralleltitel als Kopftitel mit Zweitautor und Privileg. - Drittautor unten Mitte links unter Kartenrahmen. - Maßstab unten rechts unter Titelkartusche. - Erklärungskartusche unten links
+Intermediärsprache: Deutsch  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abweichender Titel auf der Vorderseite des vorderen Banddeckels: Almanach für 1544 und 1545
+Die Vorlage enthält insgesamt 3 Werke </t>
+  </si>
+  <si>
+    <t xml:space="preserve">With: Index emendatus perfecit / J. Christian Bay
+Die Vorlage enthält insgesamt 2 Werke </t>
   </si>
   <si>
     <t xml:space="preserve">Umfang</t>
@@ -1901,7 +2188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1951,6 +2238,20 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1980,7 +2281,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2173,6 +2474,34 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2261,9 +2590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3882600</xdr:colOff>
+      <xdr:colOff>3882240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2273,7 +2602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11521440" cy="9521280"/>
+          <a:ext cx="11759400" cy="9520920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2313,14 +2642,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2603,13 +2932,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2820,15 +3149,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,15 +3361,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,15 +3573,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,15 +3785,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,15 +3999,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3898,13 +4227,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4087,13 +4416,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4257,13 +4586,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4558139534884"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,324 +4809,322 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8186046511628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5023255813953"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="B6" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-    </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-    </row>
-    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="275.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="F11" s="51"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="24" t="n">
-        <v>509133061</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>274</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="B14" s="24" t="n">
-        <v>585243190</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>276</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41" t="s">
-        <v>277</v>
-      </c>
-      <c r="B15" s="24" t="n">
-        <v>349876193</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>278</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
-        <v>279</v>
-      </c>
-      <c r="B16" s="24" t="n">
-        <v>129495476</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="B17" s="24" t="n">
-        <v>336079826</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>282</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="B18" s="24" t="n">
-        <v>787199796</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="B19" s="24" t="n">
-        <v>872316203</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>285</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41" t="s">
-        <v>273</v>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="B20" s="24" t="n">
-        <v>683536028</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>286</v>
+        <v>129993549</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>291</v>
       </c>
       <c r="D20" s="20"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41" t="s">
-        <v>287</v>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17" t="s">
+        <v>292</v>
       </c>
       <c r="B21" s="24" t="n">
-        <v>826257127</v>
-      </c>
-      <c r="C21" s="46" t="s">
+        <v>129494860</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" s="24" t="n">
+        <v>129292834</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="B23" s="24" t="n">
+        <v>329875515</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="24" t="n">
+        <v>888820720</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
+      <c r="B25" s="24" t="n">
+        <v>487757955</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #128"/>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #187"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4814,13 +5141,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.4511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5023,22 +5350,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.9767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.8046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5046,7 +5374,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5055,12 +5383,12 @@
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5069,12 +5397,12 @@
       <c r="G2" s="31"/>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5088,7 +5416,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5102,7 +5430,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5116,7 +5444,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5145,20 +5473,20 @@
       <c r="C8" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="35"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>289</v>
+        <v>235</v>
       </c>
       <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="D9" s="40"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -5203,29 +5531,29 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="B13" s="24" t="n">
-        <v>151797196</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>294</v>
+        <v>509133061</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>306</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
       <c r="F13" s="44"/>
     </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B14" s="24" t="n">
-        <v>770927416</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>295</v>
+        <v>585243190</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>308</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
@@ -5233,21 +5561,105 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="B15" s="24" t="n">
-        <v>194273989</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>297</v>
+        <v>349876193</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>310</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44"/>
     </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>129495476</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>336079826</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="44"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="41" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" s="24" t="n">
+        <v>787199796</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" s="24" t="n">
+        <v>872316203</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" s="24" t="n">
+        <v>683536028</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="B21" s="24" t="n">
+        <v>826257127</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="44"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #149"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #128"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5266,20 +5678,20 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.4558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5287,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5296,12 +5708,12 @@
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5310,12 +5722,12 @@
       <c r="G2" s="31"/>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5329,7 +5741,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5343,7 +5755,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5357,7 +5769,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5393,10 +5805,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -5444,43 +5856,43 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
       <c r="F13" s="44"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B14" s="24" t="n">
-        <v>193804867</v>
+        <v>770927416</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="43"/>
       <c r="F14" s="44"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="B15" s="24" t="n">
-        <v>409606901</v>
+        <v>194273989</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
@@ -5488,7 +5900,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #150"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #149"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5505,23 +5917,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,7 +5940,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5538,12 +5949,12 @@
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="142.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5557,7 +5968,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5571,7 +5982,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5585,7 +5996,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5599,7 +6010,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5628,18 +6039,20 @@
       <c r="C8" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="34"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="38"/>
+        <v>336</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>337</v>
+      </c>
       <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
+      <c r="D9" s="39"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -5686,21 +6099,49 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
       <c r="B13" s="24" t="n">
-        <v>233814418</v>
+        <v>151797196</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
       <c r="F13" s="44"/>
     </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>193804867</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>409606901</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="Ticket #132"/>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #150"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5717,23 +6158,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.9627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5741,7 +6182,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5750,12 +6191,12 @@
       <c r="G1" s="31"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" customFormat="false" ht="156.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>318</v>
+      <c r="B2" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5769,7 +6210,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5783,7 +6224,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5792,12 +6233,12 @@
       <c r="G4" s="31"/>
       <c r="H4" s="32"/>
     </row>
-    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>321</v>
+        <v>345</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -5811,7 +6252,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>322</v>
+        <v>346</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -5840,6 +6281,218 @@
       <c r="C8" s="34" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>233814418</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>348</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="Ticket #132"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.3162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" customFormat="false" ht="156.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="34"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
@@ -5847,13 +6500,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>323</v>
+        <v>355</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>325</v>
+        <v>357</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -5862,10 +6515,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>326</v>
+        <v>358</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -5875,10 +6528,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -5928,18 +6581,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>331</v>
+        <v>363</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44" t="s">
-        <v>332</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -5972,11 +6625,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6271,11 +6924,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6604,11 +7257,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.8232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6986,10 +7639,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.72093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7220,15 +7873,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7434,15 +8087,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7674,15 +8327,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Different transaltions, mainly lower case for english words
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1412,7 +1412,7 @@
     <t xml:space="preserve">Es werden sämtliche Verknüpfungen aus externen Quellen aus der bibliographischen Ebene (PICA 408X und 4099 in Marc unter 856) dargestellt</t>
   </si>
   <si>
-    <t xml:space="preserve">Further Information</t>
+    <t xml:space="preserve">Further information</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket 182</t>
@@ -1463,7 +1463,7 @@
     <t xml:space="preserve">Preceding Entry, Succeeding Entry</t>
   </si>
   <si>
-    <t xml:space="preserve">Preceding / Succeeding Title</t>
+    <t xml:space="preserve">Preceding / succeeding title</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket #200</t>
@@ -2590,9 +2590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3882240</xdr:colOff>
+      <xdr:colOff>3881880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,7 +2602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11759400" cy="9520920"/>
+          <a:ext cx="11987640" cy="9520560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2642,14 +2642,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="58.9488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2932,13 +2932,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3144,20 +3144,20 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,15 +3361,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,21 +3567,21 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,15 +3785,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,20 +3994,20 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4221,19 +4221,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4273,7 +4273,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4416,13 +4416,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4581,18 +4581,18 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4631,7 +4631,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4811,19 +4811,19 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8186046511628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,13 +5141,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.7906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5352,21 +5352,21 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.8046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5425,7 +5425,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="32"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5684,14 +5684,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5925,14 +5925,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6166,15 +6166,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,15 +6378,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.3162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.6837209302326"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,16 +6620,15 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.0279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6918,17 +6917,16 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.6232558139535"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7257,11 +7255,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.2883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.3953488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7633,16 +7630,15 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.0372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.2511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7873,15 +7869,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8082,20 +8078,20 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8321,21 +8317,21 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.3441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Minor fixes and unit test for title variation metadata (fixes #136)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1516,10 +1516,7 @@
     <t xml:space="preserve">Varying Form of Title, General notes, With note, </t>
   </si>
   <si>
-    <t xml:space="preserve">Anmerkungen:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes:</t>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket #187</t>
@@ -1729,15 +1726,15 @@
 500 $a</t>
   </si>
   <si>
-    <t xml:space="preserve">Hauptsacht. Anfangs: Nature and resources
+    <t xml:space="preserve">Hauptsacht. anfangs: Nature and resources
 Zusatz wechselt</t>
   </si>
   <si>
     <t xml:space="preserve">246 $i, $a</t>
   </si>
   <si>
-    <t xml:space="preserve">Nebent. : Nature, science, progrès 
-Zusatz bis 88.1960: Revue des sciences et de leurs applications  </t>
+    <t xml:space="preserve">Nebent.: Nature, science, progrès
+Zusatz bis 88.1960: Revue des sciences et de leurs applications</t>
   </si>
   <si>
     <t xml:space="preserve">246 $i, $a
@@ -1746,9 +1743,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zusatz anfangs: a weekly illustrated journal of science
-Zusatz bis 435.2005, Nr. 7039: international weekly journal of science    
+Zusatz bis 435.2005, Nr. 7039: international weekly journal of science
 Repr.: New York, NY : Johnson
-Ungezählte Beil.: The genome directory; The yeast genome directory; Suppl.; Produktschau für Deutschland; Science in Spain; Science in Latin America; Nature net guide; Nature jobs; Science &amp; technology networks in Scandinavia; Nature outlook; Nature insight; Nature publishing index  </t>
+Ungezählte Beil.: The genome directory; The yeast genome directory; Suppl.; Produktschau für Deutschland; Science in Spain; Science in Latin America; Nature net guide; Nature jobs; Science &amp; technology networks in Scandinavia; Nature outlook; Nature insight; Nature publishing index</t>
   </si>
   <si>
     <t xml:space="preserve">246 $a
@@ -1757,15 +1754,15 @@
   <si>
     <t xml:space="preserve">Parallelt.:Thuringiæ Tabula
 Titelkartusche mit allegor. Darstell. der Landwirtschaft und der Jagd unten rechts. - Paralleltitel als Kopftitel mit Zweitautor und Privileg. - Drittautor unten Mitte links unter Kartenrahmen. - Maßstab unten rechts unter Titelkartusche. - Erklärungskartusche unten links
-Intermediärsprache: Deutsch  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Abweichender Titel auf der Vorderseite des vorderen Banddeckels: Almanach für 1544 und 1545
-Die Vorlage enthält insgesamt 3 Werke </t>
+Intermediärsprache: Deutsch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abweichender Titel auf der Vorderseite des vorderen Banddeckels: Almanach für 1544 und 1545
+Die Vorlage enthält insgesamt 3 Werke</t>
   </si>
   <si>
     <t xml:space="preserve">With: Index emendatus perfecit / J. Christian Bay
-Die Vorlage enthält insgesamt 2 Werke </t>
+Die Vorlage enthält insgesamt 2 Werke</t>
   </si>
   <si>
     <t xml:space="preserve">Umfang</t>
@@ -1775,6 +1772,9 @@
   </si>
   <si>
     <t xml:space="preserve">Physical Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical description</t>
   </si>
   <si>
     <t xml:space="preserve">Ticket #128</t>
@@ -2590,9 +2590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3881880</xdr:colOff>
+      <xdr:colOff>3881520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,7 +2602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11987640" cy="9520560"/>
+          <a:ext cx="12234600" cy="9520200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2642,14 +2642,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.5023255813954"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.9906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2932,13 +2932,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3149,15 +3149,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,15 +3361,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,15 +3573,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,15 +3785,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,15 +3999,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,13 +4227,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4416,13 +4416,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4586,13 +4586,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,19 +4811,19 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,20 +4854,20 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4879,7 +4879,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4906,42 +4906,42 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="23" t="s">
         <v>275</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="275.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="C10" s="34" t="s">
         <v>278</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>280</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>281</v>
       </c>
       <c r="C11" s="50"/>
       <c r="F11" s="51"/>
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>282</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>283</v>
       </c>
       <c r="C12" s="50"/>
       <c r="E12" s="3"/>
@@ -4949,10 +4949,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>284</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>285</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="52"/>
@@ -4961,10 +4961,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="3"/>
@@ -4973,10 +4973,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>288</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>289</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="3"/>
@@ -5031,13 +5031,13 @@
     </row>
     <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B20" s="24" t="n">
         <v>129993549</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
@@ -5045,27 +5045,27 @@
     </row>
     <row r="21" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B21" s="24" t="n">
         <v>129494860</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B22" s="24" t="n">
         <v>129292834</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
@@ -5073,13 +5073,13 @@
     </row>
     <row r="23" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B23" s="24" t="n">
         <v>329875515</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
@@ -5087,13 +5087,13 @@
     </row>
     <row r="24" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B24" s="24" t="n">
         <v>888820720</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -5101,13 +5101,13 @@
     </row>
     <row r="25" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B25" s="24" t="n">
         <v>487757955</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
@@ -5141,13 +5141,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.0046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5352,21 +5352,21 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5374,7 +5374,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -5388,7 +5388,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -5402,7 +5402,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5416,7 +5416,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -5684,14 +5684,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5925,14 +5925,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6166,15 +6166,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,15 +6378,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6625,10 +6625,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.0279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6923,10 +6924,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7255,10 +7257,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.3953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7636,9 +7639,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.2511627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.5906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7869,15 +7873,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8083,15 +8087,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8323,15 +8327,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3162790697675"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Show ISBN and invalid ISBN correctly in the records metadata (fixes #170)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,8 +30,10 @@
     <sheet name="Umfang" sheetId="20" state="visible" r:id="rId21"/>
     <sheet name="Fingerprint" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Bibliographische Zitate" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="ZDB-Nummer" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="Basisklassifikation" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="ISBN" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Falsche ISBN" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="ZDB-Nummer" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Basisklassifikation" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -217,6 +219,56 @@
 </comments>
 </file>
 
+<file path=xl/comments23.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments24.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Vorgaben befinden sich in einer eigenen Tabelle
+	-Nicole Zeiler</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
@@ -318,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="386">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -1896,6 +1948,162 @@
   </si>
   <si>
     <t xml:space="preserve">IG 1281 ; GW 12189 ; ISTC ih00015000 ; BSB-Ink H-41 ; H 8426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISBN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Standard Book Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket #170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">020 $9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Verwende $9 statt $a für die Anzeige, weil es die vorlagetreue Schreibweise (mit den Bindestrichen) enthält.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $9 : $c
+           $9 : $c
+020 ist wiederholbar. Wenn mehrfach belegt, ISBN untereinander anzeigen</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">020 $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terms of availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-86025-284-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$9 und $c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">978-92-897-1568-3
+978-92-2-130471-5 : ILO
+978-92-897-1569-0 : web
+978-92-2-130472-2 : PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52680498X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-540-69713-6 : EUR 29.95, sfr 46.00
+978-3-540-69713-8 : EUR 29.95, sfr 46.00
+978-3-540-69739-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falsche ISBN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid ISBN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">020 $z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canceled/invalid ISBN</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In Solr-Marc ist die falsche ISBN leider nur ohne "-" vorhanden.
+Anzeige:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Falsche</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ISBN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> $z
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9784540697138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9783643137173</t>
   </si>
   <si>
     <t xml:space="preserve">ZDB-Nummer</t>
@@ -2281,7 +2489,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2502,6 +2710,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2590,9 +2806,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3881520</xdr:colOff>
+      <xdr:colOff>3880800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,7 +2818,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12234600" cy="9520200"/>
+          <a:ext cx="12729240" cy="9519480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2642,14 +2858,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.9906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.3441860465116"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.0372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.4093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2932,13 +3148,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3149,15 +3365,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,15 +3577,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,15 +3789,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,15 +4001,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,15 +4215,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,13 +4443,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4411,18 +4627,18 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4581,18 +4797,18 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,19 +5027,19 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.1162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.0511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,13 +5357,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.3441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5358,15 +5574,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5684,14 +5900,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5925,14 +6141,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1162790697675"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6158,6 +6374,456 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.2558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>187029679</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>884572641</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #170"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>361</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>885659430</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>362</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId2" display="Ticket #170"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6166,15 +6832,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,7 +6848,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>342</v>
+        <v>363</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6196,7 +6862,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>343</v>
+        <v>364</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6210,7 +6876,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6224,7 +6890,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>342</v>
+        <v>363</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6238,7 +6904,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6252,7 +6918,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6288,7 +6954,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
@@ -6339,13 +7005,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="B13" s="24" t="n">
         <v>233814418</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="43"/>
@@ -6365,7 +7031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -6378,15 +7044,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7162790697675"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6394,7 +7060,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -6407,8 +7073,8 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>350</v>
+      <c r="B2" s="57" t="s">
+        <v>371</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -6422,7 +7088,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>351</v>
+        <v>372</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -6436,7 +7102,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>352</v>
+        <v>373</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -6450,7 +7116,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -6464,7 +7130,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -6500,13 +7166,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>357</v>
+        <v>378</v>
       </c>
       <c r="D9" s="39"/>
       <c r="F9" s="3"/>
@@ -6515,10 +7181,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>358</v>
+        <v>379</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -6528,10 +7194,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -6581,18 +7247,18 @@
     </row>
     <row r="15" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="B15" s="24" t="n">
         <v>868759473</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>363</v>
+        <v>384</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -6625,11 +7291,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6924,11 +7590,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7257,11 +7923,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.2372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.5023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7639,10 +8305,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.5906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.5116279069767"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7873,15 +8539,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8087,15 +8753,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8327,15 +8993,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Unit tests for RecordDataFormatter work with the new versions of VuFind and PHPUnit (but still deprecation warnings)
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -2806,9 +2806,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3880800</xdr:colOff>
+      <xdr:colOff>3880440</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2818,7 +2818,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12729240" cy="9519480"/>
+          <a:ext cx="12995640" cy="9519120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2858,14 +2858,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.0372093023256"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.4093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.4976744186047"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.4976744186046"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="66.3302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3148,13 +3148,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3365,15 +3364,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,15 +3576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,15 +3788,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4001,15 +4000,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4215,15 +4214,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4443,13 +4442,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4632,13 +4630,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4802,13 +4799,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.4139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5033,13 +5030,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.0511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.0232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5357,13 +5354,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5574,15 +5570,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.2651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5900,14 +5896,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6141,14 +6137,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,19 +6372,19 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.2558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6619,13 +6615,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5627906976744"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.9162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6832,15 +6828,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7044,15 +7040,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7162790697675"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4372093023256"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7285,17 +7281,17 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7485,7 +7481,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
         <v>64</v>
       </c>
@@ -7527,7 +7523,7 @@
       <c r="E21" s="21"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17" t="s">
         <v>70</v>
       </c>
@@ -7590,11 +7586,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.7906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="62.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7923,11 +7919,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.1767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8305,10 +8301,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="86.5116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="89.0976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8539,15 +8535,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8753,15 +8749,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8993,15 +8989,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.5906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.2232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Data changed in record -> adjust test data
</commit_message>
<xml_diff>
--- a/tests/fixtures/spreadsheet/rda.xlsx
+++ b/tests/fixtures/spreadsheet/rda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Beschreibung" sheetId="1" state="visible" r:id="rId2"/>
@@ -1093,7 +1093,7 @@
     <t xml:space="preserve">683581341</t>
   </si>
   <si>
-    <t xml:space="preserve">Klemens XI. (Papst)</t>
+    <t xml:space="preserve">Klemens XI (Papst)</t>
   </si>
   <si>
     <t xml:space="preserve">700 $a und $4
@@ -2806,9 +2806,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3880440</xdr:colOff>
+      <xdr:colOff>3880080</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2818,7 +2818,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12995640" cy="9519120"/>
+          <a:ext cx="13262040" cy="9518760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2858,14 +2858,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.4976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.4976744186046"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="66.3302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="90.0837209302326"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="73.5906976744186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="77.6511627906977"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="68.2976744186047"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3148,12 +3147,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3364,15 +3364,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3576,15 +3575,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3788,15 +3786,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,15 +3997,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,15 +4210,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4442,12 +4437,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4624,18 +4620,19 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4799,13 +4796,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.7488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.8558139534884"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.7813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5030,13 +5027,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.0232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5354,12 +5351,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.5581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5570,15 +5568,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.0976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.051162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5896,14 +5893,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6137,14 +6133,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,13 +6373,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6615,13 +6610,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.9162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6828,15 +6823,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7040,15 +7034,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4372093023256"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7281,17 +7274,17 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7586,11 +7579,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="62.5162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="64.3627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7913,17 +7906,17 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.1441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.2372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.4232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8301,10 +8294,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="89.0976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="91.8046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8535,15 +8528,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8749,15 +8741,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8989,15 +8980,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.8046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="75.4372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="77.6511627906977"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>